<commit_message>
ENDELIG KAN JEG COMMITE FILEN
</commit_message>
<xml_diff>
--- a/data/SPRR/SPRR_analysesvar_samlet.xlsx
+++ b/data/SPRR/SPRR_analysesvar_samlet.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://grundfos-my.sharepoint.com/personal/102222_grundfos_com/Documents/Desktop/Speciale/data/SPRR/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B1838E2C-57DF-442F-BA8D-29F29F483C5A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="84" documentId="8_{B1838E2C-57DF-442F-BA8D-29F29F483C5A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{319A4BE3-0B00-474B-A0B2-5D1AD5500D32}"/>
   <bookViews>
-    <workbookView visibility="hidden" xWindow="4620" yWindow="4290" windowWidth="21600" windowHeight="11280" xr2:uid="{4945AC14-70B2-4790-A402-2CEEE388F912}"/>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F3BEDCAF-2F4D-48AD-8D56-F91ED459115A}"/>
-    <workbookView visibility="hidden" xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11280" xr2:uid="{B1D28580-2409-4DF1-802D-4DFBB9E40CE8}"/>
+    <workbookView visibility="hidden" xWindow="825" yWindow="1365" windowWidth="27000" windowHeight="14235" xr2:uid="{4945AC14-70B2-4790-A402-2CEEE388F912}"/>
+    <workbookView xWindow="-28890" yWindow="150" windowWidth="27000" windowHeight="14235" xr2:uid="{F3BEDCAF-2F4D-48AD-8D56-F91ED459115A}"/>
+    <workbookView visibility="hidden" xWindow="-27000" yWindow="1965" windowWidth="27000" windowHeight="14235" xr2:uid="{B1D28580-2409-4DF1-802D-4DFBB9E40CE8}"/>
   </bookViews>
   <sheets>
     <sheet name="analyse svar" sheetId="2" r:id="rId1"/>
-    <sheet name="Prøve indhold" sheetId="1" r:id="rId2"/>
+    <sheet name="analyse_R_special" sheetId="3" r:id="rId2"/>
+    <sheet name="Prøve indhold" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="32">
   <si>
     <t xml:space="preserve">prøve nr. </t>
   </si>
@@ -89,6 +90,51 @@
   <si>
     <t>&lt; 5</t>
   </si>
+  <si>
+    <t>permeat</t>
+  </si>
+  <si>
+    <t>feed</t>
+  </si>
+  <si>
+    <t>Stream</t>
+  </si>
+  <si>
+    <t>Calcium</t>
+  </si>
+  <si>
+    <t>Sodium</t>
+  </si>
+  <si>
+    <t>Chloride</t>
+  </si>
+  <si>
+    <t>Silica</t>
+  </si>
+  <si>
+    <t>Bicarbonate</t>
+  </si>
+  <si>
+    <t>Sulphate</t>
+  </si>
+  <si>
+    <t>R Ca</t>
+  </si>
+  <si>
+    <t>R Na</t>
+  </si>
+  <si>
+    <t>R Cl</t>
+  </si>
+  <si>
+    <t>R SO4</t>
+  </si>
+  <si>
+    <t>R SiO2</t>
+  </si>
+  <si>
+    <t>RHCO3</t>
+  </si>
 </sst>
 </file>
 
@@ -111,7 +157,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -148,6 +194,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -176,7 +228,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -209,9 +261,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -526,29 +582,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82F779C8-2656-402A-A797-1D4D60846A78}">
-  <dimension ref="A3:H41"/>
+  <dimension ref="A3:N41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G14" sqref="G14"/>
     </sheetView>
-    <sheetView tabSelected="1" workbookViewId="1">
-      <selection activeCell="C39" sqref="C39:F40"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="1">
+      <selection activeCell="R15" sqref="R15"/>
     </sheetView>
     <sheetView tabSelected="1" workbookViewId="2"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="11" max="11" width="11" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C3" s="24" t="s">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C3" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="24"/>
-      <c r="E3" s="24" t="s">
+      <c r="D3" s="26"/>
+      <c r="E3" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="24"/>
-    </row>
-    <row r="4" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F3" s="26"/>
+    </row>
+    <row r="4" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -558,23 +617,41 @@
       <c r="C4" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="F4" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="H4" s="28" t="s">
+        <v>28</v>
+      </c>
+      <c r="I4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="12" t="s">
+      <c r="J4" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="K4" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="H4" s="13" t="s">
+      <c r="L4" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="M4" s="13" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="N4" s="13" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="10">
         <v>1</v>
       </c>
@@ -582,13 +659,37 @@
         <v>8</v>
       </c>
       <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
+      <c r="D5" t="e">
+        <f>(1-(C6/C5))*100</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
+      <c r="F5" t="e">
+        <f>(1-(E6/E5))*100</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="G5" s="8"/>
-      <c r="H5" s="8"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H5" t="e">
+        <f>(1-(G6/G5))*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I5" s="8"/>
+      <c r="J5" t="e">
+        <f>(1-(I6/I5))*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K5" s="8"/>
+      <c r="L5" t="e">
+        <f>(1-(K6/K5))*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M5" s="8"/>
+      <c r="N5" t="e">
+        <f>(1-(M6/M5))*100</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="10">
         <v>1</v>
       </c>
@@ -601,8 +702,14 @@
       <c r="F6" s="8"/>
       <c r="G6" s="8"/>
       <c r="H6" s="8"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I6" s="8"/>
+      <c r="J6" s="8"/>
+      <c r="K6" s="8"/>
+      <c r="L6" s="8"/>
+      <c r="M6" s="8"/>
+      <c r="N6" s="8"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="10">
         <v>2</v>
       </c>
@@ -610,13 +717,37 @@
         <v>8</v>
       </c>
       <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
+      <c r="D7" t="e">
+        <f t="shared" ref="D7:F7" si="0">(1-(C8/C7))*100</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
+      <c r="F7" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
       <c r="G7" s="8"/>
-      <c r="H7" s="8"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H7" t="e">
+        <f t="shared" ref="H7" si="1">(1-(G8/G7))*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I7" s="8"/>
+      <c r="J7" t="e">
+        <f t="shared" ref="J7" si="2">(1-(I8/I7))*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K7" s="8"/>
+      <c r="L7" t="e">
+        <f t="shared" ref="L7" si="3">(1-(K8/K7))*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M7" s="8"/>
+      <c r="N7" t="e">
+        <f t="shared" ref="N7" si="4">(1-(M8/M7))*100</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="10">
         <v>2</v>
       </c>
@@ -629,8 +760,14 @@
       <c r="F8" s="8"/>
       <c r="G8" s="8"/>
       <c r="H8" s="8"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I8" s="8"/>
+      <c r="J8" s="8"/>
+      <c r="K8" s="8"/>
+      <c r="L8" s="8"/>
+      <c r="M8" s="8"/>
+      <c r="N8" s="8"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="10">
         <v>3</v>
       </c>
@@ -638,13 +775,37 @@
         <v>8</v>
       </c>
       <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
+      <c r="D9" t="e">
+        <f>(1-(C10/C9))*100</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
+      <c r="F9" t="e">
+        <f>(1-(E10/E9))*100</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H9" t="e">
+        <f>(1-(G10/G9))*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I9" s="8"/>
+      <c r="J9" t="e">
+        <f>(1-(I10/I9))*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K9" s="8"/>
+      <c r="L9" t="e">
+        <f>(1-(K10/K9))*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M9" s="8"/>
+      <c r="N9" t="e">
+        <f>(1-(M10/M9))*100</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="10">
         <v>3</v>
       </c>
@@ -657,8 +818,14 @@
       <c r="F10" s="8"/>
       <c r="G10" s="8"/>
       <c r="H10" s="8"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I10" s="8"/>
+      <c r="J10" s="8"/>
+      <c r="K10" s="8"/>
+      <c r="L10" s="8"/>
+      <c r="M10" s="8"/>
+      <c r="N10" s="8"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="10">
         <v>4</v>
       </c>
@@ -666,13 +833,37 @@
         <v>8</v>
       </c>
       <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
+      <c r="D11" t="e">
+        <f t="shared" ref="D11:F11" si="5">(1-(C12/C11))*100</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
+      <c r="F11" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
       <c r="G11" s="8"/>
-      <c r="H11" s="8"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H11" t="e">
+        <f t="shared" ref="H11" si="6">(1-(G12/G11))*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I11" s="8"/>
+      <c r="J11" t="e">
+        <f t="shared" ref="J11" si="7">(1-(I12/I11))*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K11" s="8"/>
+      <c r="L11" t="e">
+        <f t="shared" ref="L11" si="8">(1-(K12/K11))*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M11" s="8"/>
+      <c r="N11" t="e">
+        <f t="shared" ref="N11" si="9">(1-(M12/M11))*100</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="10">
         <v>4</v>
       </c>
@@ -685,8 +876,14 @@
       <c r="F12" s="8"/>
       <c r="G12" s="8"/>
       <c r="H12" s="8"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I12" s="8"/>
+      <c r="J12" s="8"/>
+      <c r="K12" s="8"/>
+      <c r="L12" s="8"/>
+      <c r="M12" s="8"/>
+      <c r="N12" s="8"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="11">
         <v>5</v>
       </c>
@@ -696,24 +893,48 @@
       <c r="C13" s="14">
         <v>5.69</v>
       </c>
-      <c r="D13" s="15">
+      <c r="D13">
+        <f>(1-(C14/C13))*100</f>
+        <v>83.304042179261856</v>
+      </c>
+      <c r="E13" s="15">
         <v>278</v>
       </c>
-      <c r="E13" s="15">
+      <c r="F13">
+        <f>(1-(E14/E13))*100</f>
+        <v>61.870503597122294</v>
+      </c>
+      <c r="G13" s="15">
         <v>170</v>
       </c>
-      <c r="F13" s="15">
+      <c r="H13">
+        <f>(1-(G14/G13))*100</f>
+        <v>4.1176470588235254</v>
+      </c>
+      <c r="I13" s="15">
         <v>463</v>
       </c>
-      <c r="G13" s="6">
+      <c r="J13" t="e">
+        <f>(1-(I14/I13))*100</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K13" s="6">
         <f>2*59.3</f>
         <v>118.6</v>
       </c>
-      <c r="H13" s="6">
+      <c r="L13">
+        <f>(1-(K14/K13))*100</f>
+        <v>23.355817875210782</v>
+      </c>
+      <c r="M13" s="6">
         <v>445</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="N13">
+        <f>(1-(M14/M13))*100</f>
+        <v>66.516853932584269</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="11">
         <v>5</v>
       </c>
@@ -723,23 +944,29 @@
       <c r="C14" s="14">
         <v>0.95</v>
       </c>
-      <c r="D14" s="15">
+      <c r="D14" s="8"/>
+      <c r="E14" s="15">
         <v>106</v>
       </c>
-      <c r="E14" s="15">
+      <c r="F14" s="8"/>
+      <c r="G14" s="15">
         <v>163</v>
       </c>
-      <c r="F14" s="15" t="s">
+      <c r="H14" s="8"/>
+      <c r="I14" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="G14" s="6">
+      <c r="J14" s="8"/>
+      <c r="K14" s="6">
         <v>90.9</v>
       </c>
-      <c r="H14" s="6">
+      <c r="L14" s="8"/>
+      <c r="M14" s="6">
         <v>149</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="N14" s="8"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="11">
         <v>6</v>
       </c>
@@ -749,24 +976,48 @@
       <c r="C15" s="14">
         <v>3.2</v>
       </c>
-      <c r="D15" s="15">
+      <c r="D15">
+        <f t="shared" ref="D15:F15" si="10">(1-(C16/C15))*100</f>
+        <v>53.437500000000007</v>
+      </c>
+      <c r="E15" s="15">
         <v>201</v>
       </c>
-      <c r="E15" s="15">
+      <c r="F15">
+        <f t="shared" si="10"/>
+        <v>50.248756218905477</v>
+      </c>
+      <c r="G15" s="15">
         <v>165</v>
       </c>
-      <c r="F15" s="15">
+      <c r="H15">
+        <f t="shared" ref="H15" si="11">(1-(G16/G15))*100</f>
+        <v>7.8787878787878736</v>
+      </c>
+      <c r="I15" s="15">
         <v>161</v>
       </c>
-      <c r="G15" s="6">
+      <c r="J15" t="e">
+        <f t="shared" ref="J15" si="12">(1-(I16/I15))*100</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K15" s="6">
         <f>59.3*2</f>
         <v>118.6</v>
       </c>
-      <c r="H15" s="6">
+      <c r="L15">
+        <f t="shared" ref="L15" si="13">(1-(K16/K15))*100</f>
+        <v>24.536256323777394</v>
+      </c>
+      <c r="M15" s="6">
         <v>428</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="N15">
+        <f t="shared" ref="N15" si="14">(1-(M16/M15))*100</f>
+        <v>65.420560747663558</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="11">
         <v>6</v>
       </c>
@@ -776,24 +1027,30 @@
       <c r="C16" s="14">
         <v>1.49</v>
       </c>
-      <c r="D16" s="15">
+      <c r="D16" s="8"/>
+      <c r="E16" s="15">
         <v>100</v>
       </c>
-      <c r="E16" s="15">
+      <c r="F16" s="8"/>
+      <c r="G16" s="15">
         <v>152</v>
       </c>
-      <c r="F16" s="15" t="s">
+      <c r="H16" s="8"/>
+      <c r="I16" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="G16" s="6">
+      <c r="J16" s="8"/>
+      <c r="K16" s="6">
         <f>89.5</f>
         <v>89.5</v>
       </c>
-      <c r="H16" s="6">
+      <c r="L16" s="8"/>
+      <c r="M16" s="6">
         <v>148</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="N16" s="8"/>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="10">
         <v>7</v>
       </c>
@@ -801,13 +1058,37 @@
         <v>8</v>
       </c>
       <c r="C17" s="8"/>
-      <c r="D17" s="8"/>
+      <c r="D17" t="e">
+        <f>(1-(C18/C17))*100</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="E17" s="8"/>
-      <c r="F17" s="8"/>
+      <c r="F17" t="e">
+        <f>(1-(E18/E17))*100</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="G17" s="8"/>
-      <c r="H17" s="8"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H17" t="e">
+        <f>(1-(G18/G17))*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I17" s="8"/>
+      <c r="J17" t="e">
+        <f>(1-(I18/I17))*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K17" s="8"/>
+      <c r="L17" t="e">
+        <f>(1-(K18/K17))*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M17" s="8"/>
+      <c r="N17" t="e">
+        <f>(1-(M18/M17))*100</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="10">
         <v>7</v>
       </c>
@@ -820,8 +1101,14 @@
       <c r="F18" s="8"/>
       <c r="G18" s="8"/>
       <c r="H18" s="8"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I18" s="8"/>
+      <c r="J18" s="8"/>
+      <c r="K18" s="8"/>
+      <c r="L18" s="8"/>
+      <c r="M18" s="8"/>
+      <c r="N18" s="8"/>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="11">
         <v>8</v>
       </c>
@@ -831,23 +1118,47 @@
       <c r="C19" s="16">
         <v>2.8</v>
       </c>
-      <c r="D19" s="17">
+      <c r="D19">
+        <f t="shared" ref="D19:F19" si="15">(1-(C20/C19))*100</f>
+        <v>58.571428571428577</v>
+      </c>
+      <c r="E19" s="17">
         <v>265</v>
       </c>
-      <c r="E19" s="17">
+      <c r="F19">
+        <f t="shared" si="15"/>
+        <v>69.433962264150949</v>
+      </c>
+      <c r="G19" s="17">
         <v>76</v>
       </c>
-      <c r="F19" s="17">
+      <c r="H19">
+        <f t="shared" ref="H19" si="16">(1-(G20/G19))*100</f>
+        <v>-2.6315789473684292</v>
+      </c>
+      <c r="I19" s="17">
         <v>553</v>
       </c>
-      <c r="G19" s="6">
+      <c r="J19" t="e">
+        <f t="shared" ref="J19" si="17">(1-(I20/I19))*100</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K19" s="6">
         <v>67.599999999999994</v>
       </c>
-      <c r="H19" s="6">
+      <c r="L19">
+        <f t="shared" ref="L19" si="18">(1-(K20/K19))*100</f>
+        <v>27.366863905325435</v>
+      </c>
+      <c r="M19" s="6">
         <v>431</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="N19">
+        <f t="shared" ref="N19" si="19">(1-(M20/M19))*100</f>
+        <v>67.285382830626446</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="11">
         <v>8</v>
       </c>
@@ -857,23 +1168,29 @@
       <c r="C20" s="16">
         <v>1.1599999999999999</v>
       </c>
-      <c r="D20" s="17">
+      <c r="D20" s="8"/>
+      <c r="E20" s="17">
         <v>81</v>
       </c>
-      <c r="E20" s="17">
+      <c r="F20" s="8"/>
+      <c r="G20" s="17">
         <v>78</v>
       </c>
-      <c r="F20" s="17" t="s">
+      <c r="H20" s="8"/>
+      <c r="I20" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="G20" s="6">
+      <c r="J20" s="8"/>
+      <c r="K20" s="6">
         <v>49.1</v>
       </c>
-      <c r="H20" s="6">
+      <c r="L20" s="8"/>
+      <c r="M20" s="6">
         <v>141</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="N20" s="8"/>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="11">
         <v>9</v>
       </c>
@@ -883,23 +1200,47 @@
       <c r="C21" s="16">
         <v>3.06</v>
       </c>
-      <c r="D21" s="17">
+      <c r="D21">
+        <f>(1-(C22/C21))*100</f>
+        <v>49.019607843137258</v>
+      </c>
+      <c r="E21" s="17">
         <v>212</v>
       </c>
-      <c r="E21" s="17">
+      <c r="F21">
+        <f>(1-(E22/E21))*100</f>
+        <v>57.075471698113198</v>
+      </c>
+      <c r="G21" s="17">
         <v>167</v>
       </c>
-      <c r="F21" s="17">
+      <c r="H21">
+        <f>(1-(G22/G21))*100</f>
+        <v>14.371257485029943</v>
+      </c>
+      <c r="I21" s="17">
         <v>160</v>
       </c>
-      <c r="G21" s="6">
+      <c r="J21" t="e">
+        <f>(1-(I22/I21))*100</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K21" s="6">
         <v>70.5</v>
       </c>
-      <c r="H21" s="6">
+      <c r="L21">
+        <f>(1-(K22/K21))*100</f>
+        <v>30.354609929078013</v>
+      </c>
+      <c r="M21" s="6">
         <v>451</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="N21">
+        <f>(1-(M22/M21))*100</f>
+        <v>72.505543237250563</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="11">
         <v>9</v>
       </c>
@@ -909,23 +1250,29 @@
       <c r="C22" s="16">
         <v>1.56</v>
       </c>
-      <c r="D22" s="17">
+      <c r="D22" s="8"/>
+      <c r="E22" s="17">
         <v>91</v>
       </c>
-      <c r="E22" s="17">
+      <c r="F22" s="8"/>
+      <c r="G22" s="17">
         <v>143</v>
       </c>
-      <c r="F22" s="17" t="s">
+      <c r="H22" s="8"/>
+      <c r="I22" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="G22" s="6">
+      <c r="J22" s="8"/>
+      <c r="K22" s="6">
         <v>49.1</v>
       </c>
-      <c r="H22" s="6">
+      <c r="L22" s="8"/>
+      <c r="M22" s="6">
         <v>124</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="N22" s="8"/>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="10">
         <v>10</v>
       </c>
@@ -933,13 +1280,37 @@
         <v>8</v>
       </c>
       <c r="C23" s="8"/>
-      <c r="D23" s="8"/>
+      <c r="D23" t="e">
+        <f t="shared" ref="D23:F23" si="20">(1-(C24/C23))*100</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="E23" s="8"/>
-      <c r="F23" s="8"/>
+      <c r="F23" t="e">
+        <f t="shared" si="20"/>
+        <v>#DIV/0!</v>
+      </c>
       <c r="G23" s="8"/>
-      <c r="H23" s="8"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H23" t="e">
+        <f t="shared" ref="H23" si="21">(1-(G24/G23))*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I23" s="8"/>
+      <c r="J23" t="e">
+        <f t="shared" ref="J23" si="22">(1-(I24/I23))*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K23" s="8"/>
+      <c r="L23" t="e">
+        <f t="shared" ref="L23" si="23">(1-(K24/K23))*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M23" s="8"/>
+      <c r="N23" t="e">
+        <f t="shared" ref="N23" si="24">(1-(M24/M23))*100</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="10">
         <v>10</v>
       </c>
@@ -952,8 +1323,14 @@
       <c r="F24" s="8"/>
       <c r="G24" s="8"/>
       <c r="H24" s="8"/>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I24" s="8"/>
+      <c r="J24" s="8"/>
+      <c r="K24" s="8"/>
+      <c r="L24" s="8"/>
+      <c r="M24" s="8"/>
+      <c r="N24" s="8"/>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="10">
         <v>11</v>
       </c>
@@ -961,13 +1338,37 @@
         <v>8</v>
       </c>
       <c r="C25" s="8"/>
-      <c r="D25" s="8"/>
+      <c r="D25" t="e">
+        <f>(1-(C26/C25))*100</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="E25" s="8"/>
-      <c r="F25" s="8"/>
+      <c r="F25" t="e">
+        <f>(1-(E26/E25))*100</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="G25" s="8"/>
-      <c r="H25" s="8"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H25" t="e">
+        <f>(1-(G26/G25))*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I25" s="8"/>
+      <c r="J25" t="e">
+        <f>(1-(I26/I25))*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K25" s="8"/>
+      <c r="L25" t="e">
+        <f>(1-(K26/K25))*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M25" s="8"/>
+      <c r="N25" t="e">
+        <f>(1-(M26/M25))*100</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" s="10">
         <v>11</v>
       </c>
@@ -980,8 +1381,14 @@
       <c r="F26" s="8"/>
       <c r="G26" s="8"/>
       <c r="H26" s="8"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I26" s="8"/>
+      <c r="J26" s="8"/>
+      <c r="K26" s="8"/>
+      <c r="L26" s="8"/>
+      <c r="M26" s="8"/>
+      <c r="N26" s="8"/>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="11">
         <v>12</v>
       </c>
@@ -991,24 +1398,48 @@
       <c r="C27" s="18">
         <v>1.98</v>
       </c>
-      <c r="D27" s="19">
+      <c r="D27">
+        <f t="shared" ref="D27:F27" si="25">(1-(C28/C27))*100</f>
+        <v>37.37373737373737</v>
+      </c>
+      <c r="E27" s="19">
         <v>212</v>
       </c>
-      <c r="E27" s="19">
+      <c r="F27">
+        <f t="shared" si="25"/>
+        <v>53.773584905660378</v>
+      </c>
+      <c r="G27" s="19">
         <v>163</v>
       </c>
-      <c r="F27" s="19">
+      <c r="H27">
+        <f t="shared" ref="H27" si="26">(1-(G28/G27))*100</f>
+        <v>1.2269938650306789</v>
+      </c>
+      <c r="I27" s="19">
         <v>153</v>
       </c>
-      <c r="G27" s="6">
+      <c r="J27" t="e">
+        <f t="shared" ref="J27" si="27">(1-(I28/I27))*100</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K27" s="6">
         <f>2*59.3</f>
         <v>118.6</v>
       </c>
-      <c r="H27" s="6">
+      <c r="L27">
+        <f t="shared" ref="L27" si="28">(1-(K28/K27))*100</f>
+        <v>33.220910623946033</v>
+      </c>
+      <c r="M27" s="6">
         <v>247</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="N27">
+        <f t="shared" ref="N27" si="29">(1-(M28/M27))*100</f>
+        <v>49.392712550607285</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" s="11">
         <v>12</v>
       </c>
@@ -1018,23 +1449,29 @@
       <c r="C28" s="18">
         <v>1.24</v>
       </c>
-      <c r="D28" s="19">
+      <c r="D28" s="8"/>
+      <c r="E28" s="19">
         <v>98</v>
       </c>
-      <c r="E28" s="19">
+      <c r="F28" s="8"/>
+      <c r="G28" s="19">
         <v>161</v>
       </c>
-      <c r="F28" s="19" t="s">
+      <c r="H28" s="8"/>
+      <c r="I28" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="G28" s="6">
+      <c r="J28" s="8"/>
+      <c r="K28" s="6">
         <v>79.2</v>
       </c>
-      <c r="H28" s="6">
+      <c r="L28" s="8"/>
+      <c r="M28" s="6">
         <v>125</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="N28" s="8"/>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" s="10">
         <v>13</v>
       </c>
@@ -1042,13 +1479,37 @@
         <v>8</v>
       </c>
       <c r="C29" s="8"/>
-      <c r="D29" s="8"/>
+      <c r="D29" t="e">
+        <f>(1-(C30/C29))*100</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="E29" s="8"/>
-      <c r="F29" s="8"/>
+      <c r="F29" t="e">
+        <f>(1-(E30/E29))*100</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="G29" s="8"/>
-      <c r="H29" s="8"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H29" t="e">
+        <f>(1-(G30/G29))*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I29" s="8"/>
+      <c r="J29" t="e">
+        <f>(1-(I30/I29))*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K29" s="8"/>
+      <c r="L29" t="e">
+        <f>(1-(K30/K29))*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M29" s="8"/>
+      <c r="N29" t="e">
+        <f>(1-(M30/M29))*100</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" s="10">
         <v>13</v>
       </c>
@@ -1061,8 +1522,14 @@
       <c r="F30" s="8"/>
       <c r="G30" s="8"/>
       <c r="H30" s="8"/>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I30" s="8"/>
+      <c r="J30" s="8"/>
+      <c r="K30" s="8"/>
+      <c r="L30" s="8"/>
+      <c r="M30" s="8"/>
+      <c r="N30" s="8"/>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" s="11">
         <v>14</v>
       </c>
@@ -1072,23 +1539,47 @@
       <c r="C31" s="20">
         <v>2.0699999999999998</v>
       </c>
-      <c r="D31" s="21">
+      <c r="D31">
+        <f t="shared" ref="D31:F31" si="30">(1-(C32/C31))*100</f>
+        <v>50.24154589371981</v>
+      </c>
+      <c r="E31" s="21">
         <v>288</v>
       </c>
-      <c r="E31" s="21">
+      <c r="F31">
+        <f t="shared" si="30"/>
+        <v>64.930555555555557</v>
+      </c>
+      <c r="G31" s="21">
         <v>168</v>
       </c>
-      <c r="F31" s="21">
+      <c r="H31">
+        <f t="shared" ref="H31" si="31">(1-(G32/G31))*100</f>
+        <v>7.1428571428571397</v>
+      </c>
+      <c r="I31" s="21">
         <v>460</v>
       </c>
-      <c r="G31" s="6">
+      <c r="J31" t="e">
+        <f t="shared" ref="J31" si="32">(1-(I32/I31))*100</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K31" s="6">
         <v>69.900000000000006</v>
       </c>
-      <c r="H31" s="6">
+      <c r="L31">
+        <f t="shared" ref="L31" si="33">(1-(K32/K31))*100</f>
+        <v>35.765379113018604</v>
+      </c>
+      <c r="M31" s="6">
         <v>433</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="N31">
+        <f t="shared" ref="N31" si="34">(1-(M32/M31))*100</f>
+        <v>72.055427251732112</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" s="11">
         <v>14</v>
       </c>
@@ -1098,23 +1589,29 @@
       <c r="C32" s="20">
         <v>1.03</v>
       </c>
-      <c r="D32" s="21">
+      <c r="D32" s="8"/>
+      <c r="E32" s="21">
         <v>101</v>
       </c>
-      <c r="E32" s="21">
+      <c r="F32" s="8"/>
+      <c r="G32" s="21">
         <v>156</v>
       </c>
-      <c r="F32" s="21" t="s">
+      <c r="H32" s="8"/>
+      <c r="I32" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="G32" s="6">
+      <c r="J32" s="8"/>
+      <c r="K32" s="6">
         <v>44.9</v>
       </c>
-      <c r="H32" s="6">
+      <c r="L32" s="8"/>
+      <c r="M32" s="6">
         <v>121</v>
       </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="N32" s="8"/>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" s="11">
         <v>15</v>
       </c>
@@ -1124,23 +1621,47 @@
       <c r="C33" s="20">
         <v>1.7</v>
       </c>
-      <c r="D33" s="21">
+      <c r="D33">
+        <f>(1-(C34/C33))*100</f>
+        <v>64.705882352941174</v>
+      </c>
+      <c r="E33" s="21">
         <v>226</v>
       </c>
-      <c r="E33" s="21">
+      <c r="F33">
+        <f>(1-(E34/E33))*100</f>
+        <v>58.407079646017699</v>
+      </c>
+      <c r="G33" s="21">
         <v>167</v>
       </c>
-      <c r="F33" s="21">
+      <c r="H33">
+        <f>(1-(G34/G33))*100</f>
+        <v>17.365269461077848</v>
+      </c>
+      <c r="I33" s="21">
         <v>234</v>
       </c>
-      <c r="G33" s="6">
+      <c r="J33" t="e">
+        <f>(1-(I34/I33))*100</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K33" s="6">
         <v>69.2</v>
       </c>
-      <c r="H33" s="6">
+      <c r="L33">
+        <f>(1-(K34/K33))*100</f>
+        <v>37.283236994219656</v>
+      </c>
+      <c r="M33" s="6">
         <v>420</v>
       </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="N33">
+        <f>(1-(M34/M33))*100</f>
+        <v>72.857142857142861</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" s="11">
         <v>15</v>
       </c>
@@ -1150,23 +1671,29 @@
       <c r="C34" s="20">
         <v>0.6</v>
       </c>
-      <c r="D34" s="21">
+      <c r="D34" s="8"/>
+      <c r="E34" s="21">
         <v>94</v>
       </c>
-      <c r="E34" s="21">
+      <c r="F34" s="8"/>
+      <c r="G34" s="21">
         <v>138</v>
       </c>
-      <c r="F34" s="21" t="s">
+      <c r="H34" s="8"/>
+      <c r="I34" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="G34" s="6">
+      <c r="J34" s="8"/>
+      <c r="K34" s="6">
         <v>43.4</v>
       </c>
-      <c r="H34" s="6">
+      <c r="L34" s="8"/>
+      <c r="M34" s="6">
         <v>114</v>
       </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="N34" s="8"/>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" s="10">
         <v>16</v>
       </c>
@@ -1174,13 +1701,37 @@
         <v>8</v>
       </c>
       <c r="C35" s="8"/>
-      <c r="D35" s="8"/>
+      <c r="D35" t="e">
+        <f t="shared" ref="D35:F35" si="35">(1-(C36/C35))*100</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="E35" s="8"/>
-      <c r="F35" s="8"/>
+      <c r="F35" t="e">
+        <f t="shared" si="35"/>
+        <v>#DIV/0!</v>
+      </c>
       <c r="G35" s="8"/>
-      <c r="H35" s="8"/>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H35" t="e">
+        <f t="shared" ref="H35" si="36">(1-(G36/G35))*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I35" s="8"/>
+      <c r="J35" t="e">
+        <f t="shared" ref="J35" si="37">(1-(I36/I35))*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K35" s="8"/>
+      <c r="L35" t="e">
+        <f t="shared" ref="L35" si="38">(1-(K36/K35))*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M35" s="8"/>
+      <c r="N35" t="e">
+        <f t="shared" ref="N35" si="39">(1-(M36/M35))*100</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" s="10">
         <v>16</v>
       </c>
@@ -1193,8 +1744,14 @@
       <c r="F36" s="8"/>
       <c r="G36" s="8"/>
       <c r="H36" s="8"/>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I36" s="8"/>
+      <c r="J36" s="8"/>
+      <c r="K36" s="8"/>
+      <c r="L36" s="8"/>
+      <c r="M36" s="8"/>
+      <c r="N36" s="8"/>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" s="10">
         <v>17</v>
       </c>
@@ -1202,13 +1759,37 @@
         <v>8</v>
       </c>
       <c r="C37" s="8"/>
-      <c r="D37" s="8"/>
+      <c r="D37" t="e">
+        <f>(1-(C38/C37))*100</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="E37" s="8"/>
-      <c r="F37" s="8"/>
+      <c r="F37" t="e">
+        <f>(1-(E38/E37))*100</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="G37" s="8"/>
-      <c r="H37" s="8"/>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H37" t="e">
+        <f>(1-(G38/G37))*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I37" s="8"/>
+      <c r="J37" t="e">
+        <f>(1-(I38/I37))*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K37" s="8"/>
+      <c r="L37" t="e">
+        <f>(1-(K38/K37))*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M37" s="8"/>
+      <c r="N37" t="e">
+        <f>(1-(M38/M37))*100</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" s="10">
         <v>17</v>
       </c>
@@ -1221,8 +1802,14 @@
       <c r="F38" s="8"/>
       <c r="G38" s="8"/>
       <c r="H38" s="8"/>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I38" s="8"/>
+      <c r="J38" s="8"/>
+      <c r="K38" s="8"/>
+      <c r="L38" s="8"/>
+      <c r="M38" s="8"/>
+      <c r="N38" s="8"/>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" s="11">
         <v>18</v>
       </c>
@@ -1232,24 +1819,48 @@
       <c r="C39" s="22">
         <v>1.7</v>
       </c>
-      <c r="D39" s="23">
+      <c r="D39">
+        <f t="shared" ref="D39:F39" si="40">(1-(C40/C39))*100</f>
+        <v>45.294117647058819</v>
+      </c>
+      <c r="E39" s="23">
         <v>231</v>
       </c>
-      <c r="E39" s="23">
+      <c r="F39">
+        <f t="shared" si="40"/>
+        <v>59.307359307359306</v>
+      </c>
+      <c r="G39" s="23">
         <v>184</v>
       </c>
-      <c r="F39" s="23">
+      <c r="H39">
+        <f t="shared" ref="H39" si="41">(1-(G40/G39))*100</f>
+        <v>18.478260869565222</v>
+      </c>
+      <c r="I39" s="23">
         <v>157</v>
       </c>
-      <c r="G39" s="6">
+      <c r="J39" t="e">
+        <f t="shared" ref="J39" si="42">(1-(I40/I39))*100</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K39" s="6">
         <f>2*59</f>
         <v>118</v>
       </c>
-      <c r="H39" s="6">
+      <c r="L39">
+        <f t="shared" ref="L39" si="43">(1-(K40/K39))*100</f>
+        <v>43.644067796610166</v>
+      </c>
+      <c r="M39" s="6">
         <v>430</v>
       </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="N39">
+        <f t="shared" ref="N39" si="44">(1-(M40/M39))*100</f>
+        <v>75.813953488372093</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40" s="11">
         <v>18</v>
       </c>
@@ -1259,23 +1870,29 @@
       <c r="C40" s="22">
         <v>0.93</v>
       </c>
-      <c r="D40" s="23">
+      <c r="D40" s="8"/>
+      <c r="E40" s="23">
         <v>94</v>
       </c>
-      <c r="E40" s="23">
+      <c r="F40" s="8"/>
+      <c r="G40" s="23">
         <v>150</v>
       </c>
-      <c r="F40" s="23" t="s">
+      <c r="H40" s="8"/>
+      <c r="I40" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="G40" s="6">
+      <c r="J40" s="8"/>
+      <c r="K40" s="6">
         <v>66.5</v>
       </c>
-      <c r="H40" s="6">
+      <c r="L40" s="8"/>
+      <c r="M40" s="6">
         <v>104</v>
       </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="N40" s="8"/>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41" s="3"/>
     </row>
   </sheetData>
@@ -1289,6 +1906,702 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C49D89CD-92FC-4300-B69C-6EFEE60A82C5}">
+  <dimension ref="A1:AK9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="P1" workbookViewId="1">
+      <selection activeCell="AK8" sqref="AK8"/>
+    </sheetView>
+    <sheetView workbookViewId="2"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="8" width="9.140625" style="24"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="B1" s="24">
+        <v>1</v>
+      </c>
+      <c r="C1" s="24">
+        <v>1</v>
+      </c>
+      <c r="D1" s="24">
+        <v>2</v>
+      </c>
+      <c r="E1" s="24">
+        <v>2</v>
+      </c>
+      <c r="F1" s="24">
+        <v>3</v>
+      </c>
+      <c r="G1" s="24">
+        <v>3</v>
+      </c>
+      <c r="H1" s="24">
+        <v>4</v>
+      </c>
+      <c r="I1" s="24">
+        <v>4</v>
+      </c>
+      <c r="J1">
+        <v>5</v>
+      </c>
+      <c r="K1">
+        <v>5</v>
+      </c>
+      <c r="L1">
+        <v>6</v>
+      </c>
+      <c r="M1">
+        <v>6</v>
+      </c>
+      <c r="N1" s="24">
+        <v>7</v>
+      </c>
+      <c r="O1" s="24">
+        <v>7</v>
+      </c>
+      <c r="P1">
+        <v>8</v>
+      </c>
+      <c r="Q1">
+        <v>8</v>
+      </c>
+      <c r="R1">
+        <v>9</v>
+      </c>
+      <c r="S1">
+        <v>9</v>
+      </c>
+      <c r="T1" s="24">
+        <v>10</v>
+      </c>
+      <c r="U1" s="24">
+        <v>10</v>
+      </c>
+      <c r="V1" s="24">
+        <v>11</v>
+      </c>
+      <c r="W1" s="24">
+        <v>11</v>
+      </c>
+      <c r="X1">
+        <v>12</v>
+      </c>
+      <c r="Y1">
+        <v>12</v>
+      </c>
+      <c r="Z1" s="24">
+        <v>13</v>
+      </c>
+      <c r="AA1" s="24">
+        <v>13</v>
+      </c>
+      <c r="AB1">
+        <v>14</v>
+      </c>
+      <c r="AC1">
+        <v>14</v>
+      </c>
+      <c r="AD1">
+        <v>15</v>
+      </c>
+      <c r="AE1">
+        <v>15</v>
+      </c>
+      <c r="AF1" s="24">
+        <v>16</v>
+      </c>
+      <c r="AG1" s="24">
+        <v>16</v>
+      </c>
+      <c r="AH1" s="24">
+        <v>17</v>
+      </c>
+      <c r="AI1" s="24">
+        <v>17</v>
+      </c>
+      <c r="AJ1">
+        <v>18</v>
+      </c>
+      <c r="AK1">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="K2" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="L2" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="M2" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="N2" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="O2" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="P2" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q2" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="R2" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="S2" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="T2" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="U2" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="V2" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="W2" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="X2" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="Y2" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="Z2" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="AA2" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="AB2" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="AC2" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="AD2" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="AE2" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="AF2" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="AG2" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="AH2" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="AI2" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="AJ2" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="AK2" s="23" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="25"/>
+      <c r="I3" s="25"/>
+      <c r="J3" s="22">
+        <v>5.69</v>
+      </c>
+      <c r="K3" s="22">
+        <v>0.95</v>
+      </c>
+      <c r="L3" s="22">
+        <v>3.2</v>
+      </c>
+      <c r="M3" s="23">
+        <v>1.49</v>
+      </c>
+      <c r="N3" s="25"/>
+      <c r="O3" s="25"/>
+      <c r="P3" s="23">
+        <v>2.8</v>
+      </c>
+      <c r="Q3" s="23">
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="R3" s="23">
+        <v>3.06</v>
+      </c>
+      <c r="S3" s="23">
+        <v>1.56</v>
+      </c>
+      <c r="T3" s="25"/>
+      <c r="U3" s="25"/>
+      <c r="V3" s="25"/>
+      <c r="W3" s="25"/>
+      <c r="X3" s="23">
+        <v>1.98</v>
+      </c>
+      <c r="Y3" s="23">
+        <v>1.24</v>
+      </c>
+      <c r="Z3" s="25"/>
+      <c r="AA3" s="25"/>
+      <c r="AB3" s="23">
+        <v>2.0699999999999998</v>
+      </c>
+      <c r="AC3" s="23">
+        <v>1.03</v>
+      </c>
+      <c r="AD3" s="23">
+        <v>1.7</v>
+      </c>
+      <c r="AE3" s="23">
+        <v>0.6</v>
+      </c>
+      <c r="AF3" s="25"/>
+      <c r="AG3" s="25"/>
+      <c r="AH3" s="25"/>
+      <c r="AI3" s="25"/>
+      <c r="AJ3" s="23">
+        <v>1.7</v>
+      </c>
+      <c r="AK3" s="23">
+        <v>0.93</v>
+      </c>
+    </row>
+    <row r="4" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="25"/>
+      <c r="C4" s="25"/>
+      <c r="D4" s="25"/>
+      <c r="E4" s="25"/>
+      <c r="F4" s="25"/>
+      <c r="G4" s="25"/>
+      <c r="H4" s="25"/>
+      <c r="I4" s="25"/>
+      <c r="J4" s="22">
+        <v>278</v>
+      </c>
+      <c r="K4" s="22">
+        <v>106</v>
+      </c>
+      <c r="L4" s="22">
+        <v>201</v>
+      </c>
+      <c r="M4" s="23">
+        <v>100</v>
+      </c>
+      <c r="N4" s="25"/>
+      <c r="O4" s="25"/>
+      <c r="P4" s="23">
+        <v>265</v>
+      </c>
+      <c r="Q4" s="23">
+        <v>81</v>
+      </c>
+      <c r="R4" s="23">
+        <v>212</v>
+      </c>
+      <c r="S4" s="23">
+        <v>91</v>
+      </c>
+      <c r="T4" s="25"/>
+      <c r="U4" s="25"/>
+      <c r="V4" s="25"/>
+      <c r="W4" s="25"/>
+      <c r="X4" s="23">
+        <v>212</v>
+      </c>
+      <c r="Y4" s="23">
+        <v>98</v>
+      </c>
+      <c r="Z4" s="25"/>
+      <c r="AA4" s="25"/>
+      <c r="AB4" s="23">
+        <v>288</v>
+      </c>
+      <c r="AC4" s="23">
+        <v>101</v>
+      </c>
+      <c r="AD4" s="23">
+        <v>226</v>
+      </c>
+      <c r="AE4" s="23">
+        <v>94</v>
+      </c>
+      <c r="AF4" s="25"/>
+      <c r="AG4" s="25"/>
+      <c r="AH4" s="25"/>
+      <c r="AI4" s="25"/>
+      <c r="AJ4" s="23">
+        <v>231</v>
+      </c>
+      <c r="AK4" s="23">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="5" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="25"/>
+      <c r="C5" s="25"/>
+      <c r="D5" s="25"/>
+      <c r="E5" s="25"/>
+      <c r="F5" s="25"/>
+      <c r="G5" s="25"/>
+      <c r="H5" s="25"/>
+      <c r="I5" s="25"/>
+      <c r="J5" s="22">
+        <v>170</v>
+      </c>
+      <c r="K5" s="22">
+        <v>163</v>
+      </c>
+      <c r="L5" s="22">
+        <v>165</v>
+      </c>
+      <c r="M5" s="23">
+        <v>152</v>
+      </c>
+      <c r="N5" s="25"/>
+      <c r="O5" s="25"/>
+      <c r="P5" s="23">
+        <v>76</v>
+      </c>
+      <c r="Q5" s="23">
+        <v>78</v>
+      </c>
+      <c r="R5" s="23">
+        <v>167</v>
+      </c>
+      <c r="S5" s="23">
+        <v>143</v>
+      </c>
+      <c r="T5" s="25"/>
+      <c r="U5" s="25"/>
+      <c r="V5" s="25"/>
+      <c r="W5" s="25"/>
+      <c r="X5" s="23">
+        <v>163</v>
+      </c>
+      <c r="Y5" s="23">
+        <v>161</v>
+      </c>
+      <c r="Z5" s="25"/>
+      <c r="AA5" s="25"/>
+      <c r="AB5" s="23">
+        <v>168</v>
+      </c>
+      <c r="AC5" s="23">
+        <v>156</v>
+      </c>
+      <c r="AD5" s="23">
+        <v>167</v>
+      </c>
+      <c r="AE5" s="23">
+        <v>138</v>
+      </c>
+      <c r="AF5" s="25"/>
+      <c r="AG5" s="25"/>
+      <c r="AH5" s="25"/>
+      <c r="AI5" s="25"/>
+      <c r="AJ5" s="23">
+        <v>184</v>
+      </c>
+      <c r="AK5" s="23">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="6" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="25"/>
+      <c r="C6" s="25"/>
+      <c r="D6" s="25"/>
+      <c r="E6" s="25"/>
+      <c r="F6" s="25"/>
+      <c r="G6" s="25"/>
+      <c r="H6" s="25"/>
+      <c r="I6" s="25"/>
+      <c r="J6" s="22">
+        <v>463</v>
+      </c>
+      <c r="K6" s="22">
+        <v>5</v>
+      </c>
+      <c r="L6" s="22">
+        <v>161</v>
+      </c>
+      <c r="M6" s="23">
+        <v>5</v>
+      </c>
+      <c r="N6" s="25"/>
+      <c r="O6" s="25"/>
+      <c r="P6" s="23">
+        <v>553</v>
+      </c>
+      <c r="Q6" s="23">
+        <v>5</v>
+      </c>
+      <c r="R6" s="23">
+        <v>160</v>
+      </c>
+      <c r="S6" s="23">
+        <v>5</v>
+      </c>
+      <c r="T6" s="25"/>
+      <c r="U6" s="25"/>
+      <c r="V6" s="25"/>
+      <c r="W6" s="25"/>
+      <c r="X6" s="23">
+        <v>153</v>
+      </c>
+      <c r="Y6" s="23">
+        <v>5</v>
+      </c>
+      <c r="Z6" s="25"/>
+      <c r="AA6" s="25"/>
+      <c r="AB6" s="23">
+        <v>460</v>
+      </c>
+      <c r="AC6" s="23">
+        <v>5</v>
+      </c>
+      <c r="AD6" s="23">
+        <v>234</v>
+      </c>
+      <c r="AE6" s="23">
+        <v>5</v>
+      </c>
+      <c r="AF6" s="25"/>
+      <c r="AG6" s="25"/>
+      <c r="AH6" s="25"/>
+      <c r="AI6" s="25"/>
+      <c r="AJ6" s="23">
+        <v>157</v>
+      </c>
+      <c r="AK6" s="23">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="25"/>
+      <c r="C7" s="25"/>
+      <c r="D7" s="25"/>
+      <c r="E7" s="25"/>
+      <c r="F7" s="25"/>
+      <c r="G7" s="25"/>
+      <c r="H7" s="25"/>
+      <c r="I7" s="25"/>
+      <c r="J7" s="22">
+        <v>118.6</v>
+      </c>
+      <c r="K7" s="22">
+        <v>90.9</v>
+      </c>
+      <c r="L7" s="22">
+        <v>118.6</v>
+      </c>
+      <c r="M7" s="23">
+        <v>89.5</v>
+      </c>
+      <c r="N7" s="25"/>
+      <c r="O7" s="25"/>
+      <c r="P7" s="23">
+        <v>67.599999999999994</v>
+      </c>
+      <c r="Q7" s="23">
+        <v>49.1</v>
+      </c>
+      <c r="R7" s="23">
+        <v>70.5</v>
+      </c>
+      <c r="S7" s="23">
+        <v>49.1</v>
+      </c>
+      <c r="T7" s="25"/>
+      <c r="U7" s="25"/>
+      <c r="V7" s="25"/>
+      <c r="W7" s="25"/>
+      <c r="X7" s="23">
+        <v>118.6</v>
+      </c>
+      <c r="Y7" s="23">
+        <v>79.2</v>
+      </c>
+      <c r="Z7" s="25"/>
+      <c r="AA7" s="25"/>
+      <c r="AB7" s="23">
+        <v>69.900000000000006</v>
+      </c>
+      <c r="AC7" s="23">
+        <v>44.9</v>
+      </c>
+      <c r="AD7" s="23">
+        <v>69.2</v>
+      </c>
+      <c r="AE7" s="23">
+        <v>43.4</v>
+      </c>
+      <c r="AF7" s="25"/>
+      <c r="AG7" s="25"/>
+      <c r="AH7" s="25"/>
+      <c r="AI7" s="25"/>
+      <c r="AJ7" s="23">
+        <v>118</v>
+      </c>
+      <c r="AK7" s="23">
+        <v>66.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="25"/>
+      <c r="C8" s="25"/>
+      <c r="D8" s="25"/>
+      <c r="E8" s="25"/>
+      <c r="F8" s="25"/>
+      <c r="G8" s="25"/>
+      <c r="H8" s="25"/>
+      <c r="I8" s="25"/>
+      <c r="J8" s="22">
+        <v>445</v>
+      </c>
+      <c r="K8" s="22">
+        <v>149</v>
+      </c>
+      <c r="L8" s="22">
+        <v>428</v>
+      </c>
+      <c r="M8" s="23">
+        <v>148</v>
+      </c>
+      <c r="N8" s="25"/>
+      <c r="O8" s="25"/>
+      <c r="P8" s="23">
+        <v>431</v>
+      </c>
+      <c r="Q8" s="23">
+        <v>141</v>
+      </c>
+      <c r="R8" s="23">
+        <v>451</v>
+      </c>
+      <c r="S8" s="23">
+        <v>124</v>
+      </c>
+      <c r="T8" s="25"/>
+      <c r="U8" s="25"/>
+      <c r="V8" s="25"/>
+      <c r="W8" s="25"/>
+      <c r="X8" s="23">
+        <v>247</v>
+      </c>
+      <c r="Y8" s="23">
+        <v>125</v>
+      </c>
+      <c r="Z8" s="25"/>
+      <c r="AA8" s="25"/>
+      <c r="AB8" s="23">
+        <v>433</v>
+      </c>
+      <c r="AC8" s="23">
+        <v>121</v>
+      </c>
+      <c r="AD8" s="23">
+        <v>420</v>
+      </c>
+      <c r="AE8" s="23">
+        <v>114</v>
+      </c>
+      <c r="AF8" s="25"/>
+      <c r="AG8" s="25"/>
+      <c r="AH8" s="25"/>
+      <c r="AI8" s="25"/>
+      <c r="AJ8" s="23">
+        <v>430</v>
+      </c>
+      <c r="AK8" s="23">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="9" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="I9" s="24"/>
+      <c r="N9" s="24"/>
+      <c r="O9" s="24"/>
+      <c r="T9" s="24"/>
+      <c r="U9" s="24"/>
+      <c r="V9" s="24"/>
+      <c r="W9" s="24"/>
+      <c r="Z9" s="24"/>
+      <c r="AA9" s="24"/>
+      <c r="AF9" s="24"/>
+      <c r="AG9" s="24"/>
+      <c r="AH9" s="24"/>
+      <c r="AI9" s="24"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67DE9CC2-1390-4757-88D3-4EDA69644CAD}">
   <dimension ref="A3:CH27"/>
   <sheetViews>
@@ -1306,18 +2619,18 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:86" x14ac:dyDescent="0.25">
-      <c r="C3" s="24" t="s">
+      <c r="C3" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="24"/>
-      <c r="E3" s="24"/>
-      <c r="F3" s="24"/>
-      <c r="G3" s="24" t="s">
+      <c r="D3" s="26"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="26"/>
+      <c r="G3" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="24"/>
-      <c r="I3" s="24"/>
-      <c r="J3" s="24"/>
+      <c r="H3" s="26"/>
+      <c r="I3" s="26"/>
+      <c r="J3" s="26"/>
     </row>
     <row r="4" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -2555,79 +3868,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10001</Type>
-    <SequenceNumber>1000</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10002</Type>
-    <SequenceNumber>1001</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10004</Type>
-    <SequenceNumber>1002</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10006</Type>
-    <SequenceNumber>1003</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-</spe:Receivers>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_dlc_DocId xmlns="add409d8-c458-45bf-bf5f-710f0ed12ba3">CY54R7KD54KC-91199970-192712</_dlc_DocId>
-    <DLCPolicyLabelLock xmlns="B9FBF822-0A65-4D1F-BC13-C27C7257EFA0" xsi:nil="true"/>
-    <DLCPolicyLabelClientValue xmlns="B9FBF822-0A65-4D1F-BC13-C27C7257EFA0" xsi:nil="true"/>
-    <_dlc_DocIdUrl xmlns="add409d8-c458-45bf-bf5f-710f0ed12ba3">
-      <Url>https://grundfos.sharepoint.com/sites/Pro-017826/_layouts/15/DocIdRedir.aspx?ID=CY54R7KD54KC-91199970-192712</Url>
-      <Description>CY54R7KD54KC-91199970-192712</Description>
-    </_dlc_DocIdUrl>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010013E660C0EEA2F44AA3B088C58E7762CB" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="5484fa9f9b42a97565e65fac7903a307">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="add409d8-c458-45bf-bf5f-710f0ed12ba3" xmlns:ns3="B9FBF822-0A65-4D1F-BC13-C27C7257EFA0" xmlns:ns4="b9fbf822-0a65-4d1f-bc13-c27c7257efa0" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="de45a4d41d0ddc6d7e8e18579ff54800" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="add409d8-c458-45bf-bf5f-710f0ed12ba3"/>
@@ -2894,34 +4134,80 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D23B5ADC-2FED-4856-AE1D-6D8A5A36E916}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10001</Type>
+    <SequenceNumber>1000</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10002</Type>
+    <SequenceNumber>1001</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10004</Type>
+    <SequenceNumber>1002</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10006</Type>
+    <SequenceNumber>1003</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+</spe:Receivers>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{51CC3469-56E6-4BF6-AD20-3A6F9B943A35}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F80D695E-02F0-4FF4-A9B6-96C7E8E5A419}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="add409d8-c458-45bf-bf5f-710f0ed12ba3"/>
-    <ds:schemaRef ds:uri="B9FBF822-0A65-4D1F-BC13-C27C7257EFA0"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_dlc_DocId xmlns="add409d8-c458-45bf-bf5f-710f0ed12ba3">CY54R7KD54KC-91199970-192712</_dlc_DocId>
+    <DLCPolicyLabelLock xmlns="B9FBF822-0A65-4D1F-BC13-C27C7257EFA0" xsi:nil="true"/>
+    <DLCPolicyLabelClientValue xmlns="B9FBF822-0A65-4D1F-BC13-C27C7257EFA0" xsi:nil="true"/>
+    <_dlc_DocIdUrl xmlns="add409d8-c458-45bf-bf5f-710f0ed12ba3">
+      <Url>https://grundfos.sharepoint.com/sites/Pro-017826/_layouts/15/DocIdRedir.aspx?ID=CY54R7KD54KC-91199970-192712</Url>
+      <Description>CY54R7KD54KC-91199970-192712</Description>
+    </_dlc_DocIdUrl>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E0D66368-F85C-4561-B8C5-570B6192D2BA}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2939,4 +4225,31 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D23B5ADC-2FED-4856-AE1D-6D8A5A36E916}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{51CC3469-56E6-4BF6-AD20-3A6F9B943A35}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F80D695E-02F0-4FF4-A9B6-96C7E8E5A419}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="add409d8-c458-45bf-bf5f-710f0ed12ba3"/>
+    <ds:schemaRef ds:uri="B9FBF822-0A65-4D1F-BC13-C27C7257EFA0"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
jeg har endelig lavet noget
</commit_message>
<xml_diff>
--- a/data/SPRR/SPRR_analysesvar_samlet.xlsx
+++ b/data/SPRR/SPRR_analysesvar_samlet.xlsx
@@ -8,16 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://grundfos-my.sharepoint.com/personal/102222_grundfos_com/Documents/Desktop/Speciale/data/SPRR/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="84" documentId="8_{B1838E2C-57DF-442F-BA8D-29F29F483C5A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{319A4BE3-0B00-474B-A0B2-5D1AD5500D32}"/>
+  <xr:revisionPtr revIDLastSave="307" documentId="8_{B1838E2C-57DF-442F-BA8D-29F29F483C5A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{540DE0EE-A052-4118-8B8B-72EF7639E7B1}"/>
   <bookViews>
-    <workbookView visibility="hidden" xWindow="825" yWindow="1365" windowWidth="27000" windowHeight="14235" xr2:uid="{4945AC14-70B2-4790-A402-2CEEE388F912}"/>
-    <workbookView xWindow="-28890" yWindow="150" windowWidth="27000" windowHeight="14235" xr2:uid="{F3BEDCAF-2F4D-48AD-8D56-F91ED459115A}"/>
-    <workbookView visibility="hidden" xWindow="-27000" yWindow="1965" windowWidth="27000" windowHeight="14235" xr2:uid="{B1D28580-2409-4DF1-802D-4DFBB9E40CE8}"/>
+    <workbookView visibility="hidden" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4945AC14-70B2-4790-A402-2CEEE388F912}"/>
+    <workbookView visibility="hidden" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{F3BEDCAF-2F4D-48AD-8D56-F91ED459115A}"/>
+    <workbookView visibility="hidden" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B1D28580-2409-4DF1-802D-4DFBB9E40CE8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{2BA11759-6010-40F7-B40A-A3F9569E799B}"/>
   </bookViews>
   <sheets>
     <sheet name="analyse svar" sheetId="2" r:id="rId1"/>
     <sheet name="analyse_R_special" sheetId="3" r:id="rId2"/>
-    <sheet name="Prøve indhold" sheetId="1" r:id="rId3"/>
+    <sheet name="Analyse_alt" sheetId="4" r:id="rId3"/>
+    <sheet name="Prøve indhold" sheetId="1" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="36">
   <si>
     <t xml:space="preserve">prøve nr. </t>
   </si>
@@ -135,6 +137,18 @@
   <si>
     <t>RHCO3</t>
   </si>
+  <si>
+    <t>Rejection</t>
+  </si>
+  <si>
+    <t>Experiment_no</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cl_ratio </t>
+  </si>
+  <si>
+    <t>Silica_content</t>
+  </si>
 </sst>
 </file>
 
@@ -228,7 +242,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -263,11 +277,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -587,10 +611,13 @@
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G14" sqref="G14"/>
     </sheetView>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="1">
-      <selection activeCell="R15" sqref="R15"/>
+    <sheetView workbookViewId="1">
+      <selection activeCell="K39" sqref="K39"/>
     </sheetView>
     <sheetView tabSelected="1" workbookViewId="2"/>
+    <sheetView workbookViewId="3">
+      <selection activeCell="C1" sqref="C1:E1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -598,16 +625,16 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="C3" s="26" t="s">
+      <c r="C3" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="26"/>
-      <c r="E3" s="26" t="s">
+      <c r="D3" s="34"/>
+      <c r="E3" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="26"/>
-    </row>
-    <row r="4" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F3" s="34"/>
+    </row>
+    <row r="4" spans="1:14" ht="23.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -617,25 +644,25 @@
       <c r="C4" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="27" t="s">
+      <c r="D4" s="26" t="s">
         <v>26</v>
       </c>
       <c r="E4" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="27" t="s">
+      <c r="F4" s="26" t="s">
         <v>27</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H4" s="28" t="s">
+      <c r="H4" s="27" t="s">
         <v>28</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="J4" s="28" t="s">
+      <c r="J4" s="27" t="s">
         <v>29</v>
       </c>
       <c r="K4" s="12" t="s">
@@ -651,179 +678,191 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="10">
+    <row r="5" spans="1:14" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="28">
         <v>1</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="8"/>
-      <c r="D5" t="e">
+      <c r="C5" s="25"/>
+      <c r="D5" s="24" t="e">
         <f>(1-(C6/C5))*100</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="E5" s="8"/>
-      <c r="F5" t="e">
+      <c r="E5" s="25"/>
+      <c r="F5" s="24" t="e">
         <f>(1-(E6/E5))*100</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G5" s="8"/>
-      <c r="H5" t="e">
+      <c r="G5" s="25"/>
+      <c r="H5" s="24" t="e">
         <f>(1-(G6/G5))*100</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="I5" s="8"/>
-      <c r="J5" t="e">
+      <c r="I5" s="25"/>
+      <c r="J5" s="24" t="e">
         <f>(1-(I6/I5))*100</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="K5" s="8"/>
-      <c r="L5" t="e">
+      <c r="K5" s="25">
+        <v>67.8</v>
+      </c>
+      <c r="L5" s="24">
         <f>(1-(K6/K5))*100</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M5" s="8"/>
-      <c r="N5" t="e">
+        <v>15.339233038348077</v>
+      </c>
+      <c r="M5" s="25"/>
+      <c r="N5" s="24" t="e">
         <f>(1-(M6/M5))*100</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="10">
+    <row r="6" spans="1:14" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="28">
         <v>1</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8"/>
-      <c r="I6" s="8"/>
-      <c r="J6" s="8"/>
-      <c r="K6" s="8"/>
-      <c r="L6" s="8"/>
-      <c r="M6" s="8"/>
-      <c r="N6" s="8"/>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" s="10">
+      <c r="C6" s="25"/>
+      <c r="D6" s="25"/>
+      <c r="E6" s="25"/>
+      <c r="F6" s="25"/>
+      <c r="G6" s="25"/>
+      <c r="H6" s="25"/>
+      <c r="I6" s="25"/>
+      <c r="J6" s="25"/>
+      <c r="K6" s="25">
+        <v>57.4</v>
+      </c>
+      <c r="L6" s="25"/>
+      <c r="M6" s="25"/>
+      <c r="N6" s="25"/>
+    </row>
+    <row r="7" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="11">
         <v>2</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="8"/>
-      <c r="D7" t="e">
+      <c r="C7" s="22"/>
+      <c r="D7" s="3" t="e">
         <f t="shared" ref="D7:F7" si="0">(1-(C8/C7))*100</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="E7" s="8"/>
-      <c r="F7" t="e">
+      <c r="E7" s="22"/>
+      <c r="F7" s="3" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="G7" s="8"/>
-      <c r="H7" t="e">
+      <c r="G7" s="22"/>
+      <c r="H7" s="3" t="e">
         <f t="shared" ref="H7" si="1">(1-(G8/G7))*100</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="I7" s="8"/>
-      <c r="J7" t="e">
+      <c r="I7" s="22"/>
+      <c r="J7" s="3" t="e">
         <f t="shared" ref="J7" si="2">(1-(I8/I7))*100</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="K7" s="8"/>
-      <c r="L7" t="e">
+      <c r="K7" s="22">
+        <v>70.400000000000006</v>
+      </c>
+      <c r="L7" s="3">
         <f t="shared" ref="L7" si="3">(1-(K8/K7))*100</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M7" s="8"/>
-      <c r="N7" t="e">
+        <v>17.613636363636374</v>
+      </c>
+      <c r="M7" s="22"/>
+      <c r="N7" s="3" t="e">
         <f t="shared" ref="N7" si="4">(1-(M8/M7))*100</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="10">
+    <row r="8" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="11">
         <v>2</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8"/>
-      <c r="I8" s="8"/>
-      <c r="J8" s="8"/>
-      <c r="K8" s="8"/>
-      <c r="L8" s="8"/>
-      <c r="M8" s="8"/>
-      <c r="N8" s="8"/>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="10">
+      <c r="C8" s="22"/>
+      <c r="D8" s="22"/>
+      <c r="E8" s="22"/>
+      <c r="F8" s="22"/>
+      <c r="G8" s="22"/>
+      <c r="H8" s="22"/>
+      <c r="I8" s="22"/>
+      <c r="J8" s="22"/>
+      <c r="K8" s="22">
+        <v>58</v>
+      </c>
+      <c r="L8" s="22"/>
+      <c r="M8" s="22"/>
+      <c r="N8" s="22"/>
+    </row>
+    <row r="9" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="11">
         <v>3</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="8"/>
-      <c r="D9" t="e">
+      <c r="C9" s="22"/>
+      <c r="D9" s="3" t="e">
         <f>(1-(C10/C9))*100</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="E9" s="8"/>
-      <c r="F9" t="e">
+      <c r="E9" s="22"/>
+      <c r="F9" s="3" t="e">
         <f>(1-(E10/E9))*100</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G9" s="8"/>
-      <c r="H9" t="e">
+      <c r="G9" s="22"/>
+      <c r="H9" s="3" t="e">
         <f>(1-(G10/G9))*100</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="I9" s="8"/>
-      <c r="J9" t="e">
+      <c r="I9" s="22"/>
+      <c r="J9" s="3" t="e">
         <f>(1-(I10/I9))*100</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="K9" s="8"/>
-      <c r="L9" t="e">
+      <c r="K9" s="22">
+        <v>72.099999999999994</v>
+      </c>
+      <c r="L9" s="3">
         <f>(1-(K10/K9))*100</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M9" s="8"/>
-      <c r="N9" t="e">
+        <v>16.643550624133141</v>
+      </c>
+      <c r="M9" s="22"/>
+      <c r="N9" s="3" t="e">
         <f>(1-(M10/M9))*100</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="10">
+    <row r="10" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="11">
         <v>3</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="8"/>
-      <c r="I10" s="8"/>
-      <c r="J10" s="8"/>
-      <c r="K10" s="8"/>
-      <c r="L10" s="8"/>
-      <c r="M10" s="8"/>
-      <c r="N10" s="8"/>
+      <c r="C10" s="22"/>
+      <c r="D10" s="22"/>
+      <c r="E10" s="22"/>
+      <c r="F10" s="22"/>
+      <c r="G10" s="22"/>
+      <c r="H10" s="22"/>
+      <c r="I10" s="22"/>
+      <c r="J10" s="22"/>
+      <c r="K10" s="22">
+        <v>60.1</v>
+      </c>
+      <c r="L10" s="22"/>
+      <c r="M10" s="22"/>
+      <c r="N10" s="22"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="10">
@@ -1330,63 +1369,69 @@
       <c r="M24" s="8"/>
       <c r="N24" s="8"/>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A25" s="10">
+    <row r="25" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="11">
         <v>11</v>
       </c>
-      <c r="B25" s="9" t="s">
+      <c r="B25" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C25" s="8"/>
-      <c r="D25" t="e">
+      <c r="C25" s="22"/>
+      <c r="D25" s="3" t="e">
         <f>(1-(C26/C25))*100</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="E25" s="8"/>
-      <c r="F25" t="e">
+      <c r="E25" s="22"/>
+      <c r="F25" s="3" t="e">
         <f>(1-(E26/E25))*100</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G25" s="8"/>
-      <c r="H25" t="e">
+      <c r="G25" s="22"/>
+      <c r="H25" s="3" t="e">
         <f>(1-(G26/G25))*100</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="I25" s="8"/>
-      <c r="J25" t="e">
+      <c r="I25" s="22"/>
+      <c r="J25" s="3" t="e">
         <f>(1-(I26/I25))*100</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="K25" s="8"/>
-      <c r="L25" t="e">
+      <c r="K25" s="22">
+        <f>2*61.5</f>
+        <v>123</v>
+      </c>
+      <c r="L25" s="3">
         <f>(1-(K26/K25))*100</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M25" s="8"/>
-      <c r="N25" t="e">
+        <v>29.837398373983739</v>
+      </c>
+      <c r="M25" s="22"/>
+      <c r="N25" s="3" t="e">
         <f>(1-(M26/M25))*100</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A26" s="10">
+    <row r="26" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="11">
         <v>11</v>
       </c>
-      <c r="B26" s="9" t="s">
+      <c r="B26" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C26" s="8"/>
-      <c r="D26" s="8"/>
-      <c r="E26" s="8"/>
-      <c r="F26" s="8"/>
-      <c r="G26" s="8"/>
-      <c r="H26" s="8"/>
-      <c r="I26" s="8"/>
-      <c r="J26" s="8"/>
-      <c r="K26" s="8"/>
-      <c r="L26" s="8"/>
-      <c r="M26" s="8"/>
-      <c r="N26" s="8"/>
+      <c r="C26" s="22"/>
+      <c r="D26" s="22"/>
+      <c r="E26" s="22"/>
+      <c r="F26" s="22"/>
+      <c r="G26" s="22"/>
+      <c r="H26" s="22"/>
+      <c r="I26" s="22"/>
+      <c r="J26" s="22"/>
+      <c r="K26" s="22">
+        <f>86.3</f>
+        <v>86.3</v>
+      </c>
+      <c r="L26" s="22"/>
+      <c r="M26" s="22"/>
+      <c r="N26" s="22"/>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="11">
@@ -1751,63 +1796,68 @@
       <c r="M36" s="8"/>
       <c r="N36" s="8"/>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A37" s="10">
+    <row r="37" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="11">
         <v>17</v>
       </c>
-      <c r="B37" s="9" t="s">
+      <c r="B37" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C37" s="8"/>
-      <c r="D37" t="e">
+      <c r="C37" s="22"/>
+      <c r="D37" s="3" t="e">
         <f>(1-(C38/C37))*100</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="E37" s="8"/>
-      <c r="F37" t="e">
+      <c r="E37" s="22"/>
+      <c r="F37" s="3" t="e">
         <f>(1-(E38/E37))*100</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G37" s="8"/>
-      <c r="H37" t="e">
+      <c r="G37" s="22"/>
+      <c r="H37" s="3" t="e">
         <f>(1-(G38/G37))*100</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="I37" s="8"/>
-      <c r="J37" t="e">
+      <c r="I37" s="22"/>
+      <c r="J37" s="3" t="e">
         <f>(1-(I38/I37))*100</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="K37" s="8"/>
-      <c r="L37" t="e">
+      <c r="K37" s="22">
+        <f>2*61.1</f>
+        <v>122.2</v>
+      </c>
+      <c r="L37" s="3">
         <f>(1-(K38/K37))*100</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M37" s="8"/>
-      <c r="N37" t="e">
+        <v>37.234042553191493</v>
+      </c>
+      <c r="M37" s="22"/>
+      <c r="N37" s="3" t="e">
         <f>(1-(M38/M37))*100</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A38" s="10">
+    <row r="38" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="11">
         <v>17</v>
       </c>
-      <c r="B38" s="9" t="s">
+      <c r="B38" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C38" s="8"/>
-      <c r="D38" s="8"/>
-      <c r="E38" s="8"/>
-      <c r="F38" s="8"/>
-      <c r="G38" s="8"/>
-      <c r="H38" s="8"/>
-      <c r="I38" s="8"/>
-      <c r="J38" s="8"/>
-      <c r="K38" s="8"/>
-      <c r="L38" s="8"/>
-      <c r="M38" s="8"/>
-      <c r="N38" s="8"/>
+      <c r="C38" s="22"/>
+      <c r="D38" s="22"/>
+      <c r="E38" s="22"/>
+      <c r="F38" s="22"/>
+      <c r="G38" s="22"/>
+      <c r="H38" s="22"/>
+      <c r="I38" s="22"/>
+      <c r="J38" s="22"/>
+      <c r="K38" s="22">
+        <v>76.7</v>
+      </c>
+      <c r="L38" s="22"/>
+      <c r="M38" s="22"/>
+      <c r="N38" s="22"/>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" s="11">
@@ -1910,33 +1960,37 @@
   <dimension ref="A1:AK9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView topLeftCell="P1" workbookViewId="1">
-      <selection activeCell="AK8" sqref="AK8"/>
+    <sheetView tabSelected="1" workbookViewId="1">
+      <selection activeCell="AI8" sqref="AI8"/>
     </sheetView>
     <sheetView workbookViewId="2"/>
+    <sheetView workbookViewId="3"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="8" width="9.140625" style="24"/>
+    <col min="2" max="7" width="9.140625" style="3"/>
+    <col min="8" max="8" width="9.140625" style="24"/>
+    <col min="22" max="23" width="9.140625" style="3"/>
+    <col min="34" max="35" width="9.140625" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="B1" s="24">
+      <c r="B1" s="3">
         <v>1</v>
       </c>
-      <c r="C1" s="24">
+      <c r="C1" s="3">
         <v>1</v>
       </c>
-      <c r="D1" s="24">
+      <c r="D1" s="3">
         <v>2</v>
       </c>
-      <c r="E1" s="24">
+      <c r="E1" s="3">
         <v>2</v>
       </c>
-      <c r="F1" s="24">
+      <c r="F1" s="3">
         <v>3</v>
       </c>
-      <c r="G1" s="24">
+      <c r="G1" s="3">
         <v>3</v>
       </c>
       <c r="H1" s="24">
@@ -1981,10 +2035,10 @@
       <c r="U1" s="24">
         <v>10</v>
       </c>
-      <c r="V1" s="24">
+      <c r="V1" s="3">
         <v>11</v>
       </c>
-      <c r="W1" s="24">
+      <c r="W1" s="3">
         <v>11</v>
       </c>
       <c r="X1">
@@ -2017,10 +2071,10 @@
       <c r="AG1" s="24">
         <v>16</v>
       </c>
-      <c r="AH1" s="24">
+      <c r="AH1" s="3">
         <v>17</v>
       </c>
-      <c r="AI1" s="24">
+      <c r="AI1" s="3">
         <v>17</v>
       </c>
       <c r="AJ1">
@@ -2034,22 +2088,22 @@
       <c r="A2" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="25" t="s">
+      <c r="C2" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="25" t="s">
+      <c r="D2" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="25" t="s">
+      <c r="E2" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="25" t="s">
+      <c r="F2" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="G2" s="25" t="s">
+      <c r="G2" s="22" t="s">
         <v>17</v>
       </c>
       <c r="H2" s="25" t="s">
@@ -2094,10 +2148,10 @@
       <c r="U2" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="V2" s="25" t="s">
+      <c r="V2" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="W2" s="25" t="s">
+      <c r="W2" s="22" t="s">
         <v>17</v>
       </c>
       <c r="X2" s="23" t="s">
@@ -2130,10 +2184,10 @@
       <c r="AG2" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="AH2" s="25" t="s">
+      <c r="AH2" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="AI2" s="25" t="s">
+      <c r="AI2" s="22" t="s">
         <v>17</v>
       </c>
       <c r="AJ2" s="23" t="s">
@@ -2147,12 +2201,12 @@
       <c r="A3" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="25"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
+      <c r="B3" s="22"/>
+      <c r="C3" s="22"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="22"/>
+      <c r="G3" s="22"/>
       <c r="H3" s="25"/>
       <c r="I3" s="25"/>
       <c r="J3" s="22">
@@ -2183,8 +2237,8 @@
       </c>
       <c r="T3" s="25"/>
       <c r="U3" s="25"/>
-      <c r="V3" s="25"/>
-      <c r="W3" s="25"/>
+      <c r="V3" s="22"/>
+      <c r="W3" s="22"/>
       <c r="X3" s="23">
         <v>1.98</v>
       </c>
@@ -2207,8 +2261,8 @@
       </c>
       <c r="AF3" s="25"/>
       <c r="AG3" s="25"/>
-      <c r="AH3" s="25"/>
-      <c r="AI3" s="25"/>
+      <c r="AH3" s="22"/>
+      <c r="AI3" s="22"/>
       <c r="AJ3" s="23">
         <v>1.7</v>
       </c>
@@ -2220,12 +2274,12 @@
       <c r="A4" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="25"/>
-      <c r="C4" s="25"/>
-      <c r="D4" s="25"/>
-      <c r="E4" s="25"/>
-      <c r="F4" s="25"/>
-      <c r="G4" s="25"/>
+      <c r="B4" s="22"/>
+      <c r="C4" s="22"/>
+      <c r="D4" s="22"/>
+      <c r="E4" s="22"/>
+      <c r="F4" s="22"/>
+      <c r="G4" s="22"/>
       <c r="H4" s="25"/>
       <c r="I4" s="25"/>
       <c r="J4" s="22">
@@ -2256,8 +2310,8 @@
       </c>
       <c r="T4" s="25"/>
       <c r="U4" s="25"/>
-      <c r="V4" s="25"/>
-      <c r="W4" s="25"/>
+      <c r="V4" s="22"/>
+      <c r="W4" s="22"/>
       <c r="X4" s="23">
         <v>212</v>
       </c>
@@ -2280,8 +2334,8 @@
       </c>
       <c r="AF4" s="25"/>
       <c r="AG4" s="25"/>
-      <c r="AH4" s="25"/>
-      <c r="AI4" s="25"/>
+      <c r="AH4" s="22"/>
+      <c r="AI4" s="22"/>
       <c r="AJ4" s="23">
         <v>231</v>
       </c>
@@ -2293,12 +2347,12 @@
       <c r="A5" t="s">
         <v>22</v>
       </c>
-      <c r="B5" s="25"/>
-      <c r="C5" s="25"/>
-      <c r="D5" s="25"/>
-      <c r="E5" s="25"/>
-      <c r="F5" s="25"/>
-      <c r="G5" s="25"/>
+      <c r="B5" s="22"/>
+      <c r="C5" s="22"/>
+      <c r="D5" s="22"/>
+      <c r="E5" s="22"/>
+      <c r="F5" s="22"/>
+      <c r="G5" s="22"/>
       <c r="H5" s="25"/>
       <c r="I5" s="25"/>
       <c r="J5" s="22">
@@ -2329,8 +2383,8 @@
       </c>
       <c r="T5" s="25"/>
       <c r="U5" s="25"/>
-      <c r="V5" s="25"/>
-      <c r="W5" s="25"/>
+      <c r="V5" s="22"/>
+      <c r="W5" s="22"/>
       <c r="X5" s="23">
         <v>163</v>
       </c>
@@ -2353,8 +2407,8 @@
       </c>
       <c r="AF5" s="25"/>
       <c r="AG5" s="25"/>
-      <c r="AH5" s="25"/>
-      <c r="AI5" s="25"/>
+      <c r="AH5" s="22"/>
+      <c r="AI5" s="22"/>
       <c r="AJ5" s="23">
         <v>184</v>
       </c>
@@ -2366,12 +2420,12 @@
       <c r="A6" t="s">
         <v>25</v>
       </c>
-      <c r="B6" s="25"/>
-      <c r="C6" s="25"/>
-      <c r="D6" s="25"/>
-      <c r="E6" s="25"/>
-      <c r="F6" s="25"/>
-      <c r="G6" s="25"/>
+      <c r="B6" s="22"/>
+      <c r="C6" s="22"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="22"/>
+      <c r="F6" s="22"/>
+      <c r="G6" s="22"/>
       <c r="H6" s="25"/>
       <c r="I6" s="25"/>
       <c r="J6" s="22">
@@ -2402,8 +2456,8 @@
       </c>
       <c r="T6" s="25"/>
       <c r="U6" s="25"/>
-      <c r="V6" s="25"/>
-      <c r="W6" s="25"/>
+      <c r="V6" s="22"/>
+      <c r="W6" s="22"/>
       <c r="X6" s="23">
         <v>153</v>
       </c>
@@ -2426,8 +2480,8 @@
       </c>
       <c r="AF6" s="25"/>
       <c r="AG6" s="25"/>
-      <c r="AH6" s="25"/>
-      <c r="AI6" s="25"/>
+      <c r="AH6" s="22"/>
+      <c r="AI6" s="22"/>
       <c r="AJ6" s="23">
         <v>157</v>
       </c>
@@ -2439,12 +2493,24 @@
       <c r="A7" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="25"/>
-      <c r="C7" s="25"/>
-      <c r="D7" s="25"/>
-      <c r="E7" s="25"/>
-      <c r="F7" s="25"/>
-      <c r="G7" s="25"/>
+      <c r="B7" s="22">
+        <v>67.8</v>
+      </c>
+      <c r="C7" s="22">
+        <v>57.4</v>
+      </c>
+      <c r="D7" s="22">
+        <v>70.400000000000006</v>
+      </c>
+      <c r="E7" s="22">
+        <v>58</v>
+      </c>
+      <c r="F7" s="22">
+        <v>72.099999999999994</v>
+      </c>
+      <c r="G7" s="22">
+        <v>60.1</v>
+      </c>
       <c r="H7" s="25"/>
       <c r="I7" s="25"/>
       <c r="J7" s="22">
@@ -2475,8 +2541,12 @@
       </c>
       <c r="T7" s="25"/>
       <c r="U7" s="25"/>
-      <c r="V7" s="25"/>
-      <c r="W7" s="25"/>
+      <c r="V7" s="22">
+        <v>123</v>
+      </c>
+      <c r="W7" s="22">
+        <v>86.3</v>
+      </c>
       <c r="X7" s="23">
         <v>118.6</v>
       </c>
@@ -2499,8 +2569,12 @@
       </c>
       <c r="AF7" s="25"/>
       <c r="AG7" s="25"/>
-      <c r="AH7" s="25"/>
-      <c r="AI7" s="25"/>
+      <c r="AH7" s="22">
+        <v>122.2</v>
+      </c>
+      <c r="AI7" s="22">
+        <v>76.7</v>
+      </c>
       <c r="AJ7" s="23">
         <v>118</v>
       </c>
@@ -2512,12 +2586,12 @@
       <c r="A8" t="s">
         <v>24</v>
       </c>
-      <c r="B8" s="25"/>
-      <c r="C8" s="25"/>
-      <c r="D8" s="25"/>
-      <c r="E8" s="25"/>
-      <c r="F8" s="25"/>
-      <c r="G8" s="25"/>
+      <c r="B8" s="22"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="22"/>
+      <c r="E8" s="22"/>
+      <c r="F8" s="22"/>
+      <c r="G8" s="22"/>
       <c r="H8" s="25"/>
       <c r="I8" s="25"/>
       <c r="J8" s="22">
@@ -2548,8 +2622,8 @@
       </c>
       <c r="T8" s="25"/>
       <c r="U8" s="25"/>
-      <c r="V8" s="25"/>
-      <c r="W8" s="25"/>
+      <c r="V8" s="22"/>
+      <c r="W8" s="22"/>
       <c r="X8" s="23">
         <v>247</v>
       </c>
@@ -2572,8 +2646,8 @@
       </c>
       <c r="AF8" s="25"/>
       <c r="AG8" s="25"/>
-      <c r="AH8" s="25"/>
-      <c r="AI8" s="25"/>
+      <c r="AH8" s="22"/>
+      <c r="AI8" s="22"/>
       <c r="AJ8" s="23">
         <v>430</v>
       </c>
@@ -2587,14 +2661,10 @@
       <c r="O9" s="24"/>
       <c r="T9" s="24"/>
       <c r="U9" s="24"/>
-      <c r="V9" s="24"/>
-      <c r="W9" s="24"/>
       <c r="Z9" s="24"/>
       <c r="AA9" s="24"/>
       <c r="AF9" s="24"/>
       <c r="AG9" s="24"/>
-      <c r="AH9" s="24"/>
-      <c r="AI9" s="24"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2602,6 +2672,1849 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EA13149-3F9C-4F1B-BA19-91C6BCB20171}">
+  <dimension ref="A1:K56"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="2"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="3">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J2" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="K2" s="13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="28">
+        <v>1</v>
+      </c>
+      <c r="B3" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="31">
+        <v>25</v>
+      </c>
+      <c r="D3" s="31">
+        <v>75</v>
+      </c>
+      <c r="E3" s="31">
+        <v>9.25</v>
+      </c>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="25"/>
+      <c r="I3" s="25"/>
+      <c r="J3" s="25">
+        <v>67.8</v>
+      </c>
+      <c r="K3" s="25"/>
+    </row>
+    <row r="4" spans="1:11" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="28">
+        <v>1</v>
+      </c>
+      <c r="B4" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="31">
+        <v>25</v>
+      </c>
+      <c r="D4" s="31">
+        <v>75</v>
+      </c>
+      <c r="E4" s="31">
+        <v>9.25</v>
+      </c>
+      <c r="F4" s="25"/>
+      <c r="G4" s="25"/>
+      <c r="H4" s="25"/>
+      <c r="I4" s="25"/>
+      <c r="J4" s="25">
+        <v>57.4</v>
+      </c>
+      <c r="K4" s="25"/>
+    </row>
+    <row r="5" spans="1:11" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="28">
+        <v>1</v>
+      </c>
+      <c r="B5" s="29" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" s="31">
+        <v>25</v>
+      </c>
+      <c r="D5" s="31">
+        <v>75</v>
+      </c>
+      <c r="E5" s="31">
+        <v>9.25</v>
+      </c>
+      <c r="F5" s="25" t="e">
+        <f t="shared" ref="F5:I5" si="0">(1-(F4/F3))*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G5" s="25" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H5" s="25" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I5" s="25" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J5" s="25">
+        <f>(1-(J4/J3))*100</f>
+        <v>15.339233038348077</v>
+      </c>
+      <c r="K5" s="25" t="e">
+        <f>(1-(K4/K3))*100</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="11">
+        <v>2</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="32">
+        <v>50</v>
+      </c>
+      <c r="D6" s="32">
+        <v>75</v>
+      </c>
+      <c r="E6" s="32">
+        <v>9.25</v>
+      </c>
+      <c r="F6" s="22"/>
+      <c r="G6" s="22"/>
+      <c r="H6" s="22"/>
+      <c r="I6" s="22"/>
+      <c r="J6" s="22">
+        <v>70.400000000000006</v>
+      </c>
+      <c r="K6" s="22"/>
+    </row>
+    <row r="7" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="11">
+        <v>2</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="32">
+        <v>50</v>
+      </c>
+      <c r="D7" s="32">
+        <v>75</v>
+      </c>
+      <c r="E7" s="32">
+        <v>9.25</v>
+      </c>
+      <c r="F7" s="22"/>
+      <c r="G7" s="22"/>
+      <c r="H7" s="22"/>
+      <c r="I7" s="22"/>
+      <c r="J7" s="22">
+        <v>58</v>
+      </c>
+      <c r="K7" s="22"/>
+    </row>
+    <row r="8" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="11">
+        <v>2</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" s="32">
+        <v>50</v>
+      </c>
+      <c r="D8" s="32">
+        <v>75</v>
+      </c>
+      <c r="E8" s="32">
+        <v>9.25</v>
+      </c>
+      <c r="F8" s="22" t="e">
+        <f t="shared" ref="F8" si="1">(1-(F7/F6))*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G8" s="22" t="e">
+        <f t="shared" ref="G8" si="2">(1-(G7/G6))*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H8" s="22" t="e">
+        <f t="shared" ref="H8" si="3">(1-(H7/H6))*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I8" s="22" t="e">
+        <f t="shared" ref="I8" si="4">(1-(I7/I6))*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J8" s="22">
+        <f>(1-(J7/J6))*100</f>
+        <v>17.613636363636374</v>
+      </c>
+      <c r="K8" s="22" t="e">
+        <f>(1-(K7/K6))*100</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="11">
+        <v>3</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="32">
+        <v>75</v>
+      </c>
+      <c r="D9" s="32">
+        <v>75</v>
+      </c>
+      <c r="E9" s="32">
+        <v>9.25</v>
+      </c>
+      <c r="F9" s="22"/>
+      <c r="G9" s="22"/>
+      <c r="H9" s="22"/>
+      <c r="I9" s="22"/>
+      <c r="J9" s="22">
+        <v>72.099999999999994</v>
+      </c>
+      <c r="K9" s="22"/>
+    </row>
+    <row r="10" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="11">
+        <v>3</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="32">
+        <v>75</v>
+      </c>
+      <c r="D10" s="32">
+        <v>75</v>
+      </c>
+      <c r="E10" s="32">
+        <v>9.25</v>
+      </c>
+      <c r="F10" s="22"/>
+      <c r="G10" s="22"/>
+      <c r="H10" s="22"/>
+      <c r="I10" s="22"/>
+      <c r="J10" s="22">
+        <v>60.1</v>
+      </c>
+      <c r="K10" s="22"/>
+    </row>
+    <row r="11" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="11">
+        <v>3</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="32">
+        <v>75</v>
+      </c>
+      <c r="D11" s="32">
+        <v>75</v>
+      </c>
+      <c r="E11" s="32">
+        <v>9.25</v>
+      </c>
+      <c r="F11" s="22" t="e">
+        <f t="shared" ref="F11" si="5">(1-(F10/F9))*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G11" s="22" t="e">
+        <f t="shared" ref="G11" si="6">(1-(G10/G9))*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H11" s="22" t="e">
+        <f t="shared" ref="H11" si="7">(1-(H10/H9))*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I11" s="22" t="e">
+        <f t="shared" ref="I11" si="8">(1-(I10/I9))*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J11" s="22">
+        <f>(1-(J10/J9))*100</f>
+        <v>16.643550624133141</v>
+      </c>
+      <c r="K11" s="22" t="e">
+        <f>(1-(K10/K9))*100</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="10">
+        <v>4</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="33">
+        <v>25</v>
+      </c>
+      <c r="D12" s="33">
+        <v>125</v>
+      </c>
+      <c r="E12" s="33">
+        <v>9.25</v>
+      </c>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="8"/>
+      <c r="I12" s="8"/>
+      <c r="J12" s="8"/>
+      <c r="K12" s="8"/>
+    </row>
+    <row r="13" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="10">
+        <v>4</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="33">
+        <v>25</v>
+      </c>
+      <c r="D13" s="33">
+        <v>125</v>
+      </c>
+      <c r="E13" s="33">
+        <v>9.25</v>
+      </c>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="8"/>
+      <c r="I13" s="8"/>
+      <c r="J13" s="8"/>
+      <c r="K13" s="8"/>
+    </row>
+    <row r="14" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="10">
+        <v>4</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C14" s="33">
+        <v>25</v>
+      </c>
+      <c r="D14" s="33">
+        <v>125</v>
+      </c>
+      <c r="E14" s="33">
+        <v>9.25</v>
+      </c>
+      <c r="F14" s="8" t="e">
+        <f t="shared" ref="F14" si="9">(1-(F13/F12))*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G14" s="8" t="e">
+        <f t="shared" ref="G14" si="10">(1-(G13/G12))*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H14" s="8" t="e">
+        <f t="shared" ref="H14" si="11">(1-(H13/H12))*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I14" s="8" t="e">
+        <f t="shared" ref="I14" si="12">(1-(I13/I12))*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J14" s="8" t="e">
+        <f>(1-(J13/J12))*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K14" s="8" t="e">
+        <f>(1-(K13/K12))*100</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="11">
+        <v>5</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" s="32">
+        <v>50</v>
+      </c>
+      <c r="D15" s="32">
+        <v>125</v>
+      </c>
+      <c r="E15" s="32">
+        <v>9.25</v>
+      </c>
+      <c r="F15" s="22">
+        <v>5.69</v>
+      </c>
+      <c r="G15" s="22">
+        <v>278</v>
+      </c>
+      <c r="H15" s="22">
+        <v>170</v>
+      </c>
+      <c r="I15" s="22">
+        <v>463</v>
+      </c>
+      <c r="J15" s="22">
+        <f>2*59.3</f>
+        <v>118.6</v>
+      </c>
+      <c r="K15" s="22">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="11">
+        <v>5</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" s="32">
+        <v>50</v>
+      </c>
+      <c r="D16" s="32">
+        <v>125</v>
+      </c>
+      <c r="E16" s="32">
+        <v>9.25</v>
+      </c>
+      <c r="F16" s="22">
+        <v>0.95</v>
+      </c>
+      <c r="G16" s="22">
+        <v>106</v>
+      </c>
+      <c r="H16" s="22">
+        <v>163</v>
+      </c>
+      <c r="I16" s="22">
+        <v>5</v>
+      </c>
+      <c r="J16" s="22">
+        <v>90.9</v>
+      </c>
+      <c r="K16" s="22">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="11">
+        <v>5</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C17" s="32">
+        <v>50</v>
+      </c>
+      <c r="D17" s="32">
+        <v>125</v>
+      </c>
+      <c r="E17" s="32">
+        <v>9.25</v>
+      </c>
+      <c r="F17" s="22">
+        <f t="shared" ref="F17" si="13">(1-(F16/F15))*100</f>
+        <v>83.304042179261856</v>
+      </c>
+      <c r="G17" s="22">
+        <f t="shared" ref="G17" si="14">(1-(G16/G15))*100</f>
+        <v>61.870503597122294</v>
+      </c>
+      <c r="H17" s="22">
+        <f t="shared" ref="H17" si="15">(1-(H16/H15))*100</f>
+        <v>4.1176470588235254</v>
+      </c>
+      <c r="I17" s="22">
+        <f t="shared" ref="I17" si="16">(1-(I16/I15))*100</f>
+        <v>98.920086393088553</v>
+      </c>
+      <c r="J17" s="22">
+        <f>(1-(J16/J15))*100</f>
+        <v>23.355817875210782</v>
+      </c>
+      <c r="K17" s="22">
+        <f>(1-(K16/K15))*100</f>
+        <v>66.516853932584269</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="11">
+        <v>6</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" s="32">
+        <v>75</v>
+      </c>
+      <c r="D18" s="32">
+        <v>125</v>
+      </c>
+      <c r="E18" s="32">
+        <v>9.25</v>
+      </c>
+      <c r="F18" s="22">
+        <v>3.2</v>
+      </c>
+      <c r="G18" s="22">
+        <v>201</v>
+      </c>
+      <c r="H18" s="22">
+        <v>165</v>
+      </c>
+      <c r="I18" s="22">
+        <v>161</v>
+      </c>
+      <c r="J18" s="22">
+        <f>59.3*2</f>
+        <v>118.6</v>
+      </c>
+      <c r="K18" s="22">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="11">
+        <v>6</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19" s="32">
+        <v>75</v>
+      </c>
+      <c r="D19" s="32">
+        <v>125</v>
+      </c>
+      <c r="E19" s="32">
+        <v>9.25</v>
+      </c>
+      <c r="F19" s="22">
+        <v>1.49</v>
+      </c>
+      <c r="G19" s="22">
+        <v>100</v>
+      </c>
+      <c r="H19" s="22">
+        <v>152</v>
+      </c>
+      <c r="I19" s="22">
+        <v>5</v>
+      </c>
+      <c r="J19" s="22">
+        <f>89.5</f>
+        <v>89.5</v>
+      </c>
+      <c r="K19" s="22">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="11">
+        <v>6</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C20" s="32">
+        <v>75</v>
+      </c>
+      <c r="D20" s="32">
+        <v>125</v>
+      </c>
+      <c r="E20" s="32">
+        <v>9.25</v>
+      </c>
+      <c r="F20" s="22">
+        <f t="shared" ref="F20" si="17">(1-(F19/F18))*100</f>
+        <v>53.437500000000007</v>
+      </c>
+      <c r="G20" s="22">
+        <f t="shared" ref="G20" si="18">(1-(G19/G18))*100</f>
+        <v>50.248756218905477</v>
+      </c>
+      <c r="H20" s="22">
+        <f t="shared" ref="H20" si="19">(1-(H19/H18))*100</f>
+        <v>7.8787878787878736</v>
+      </c>
+      <c r="I20" s="22">
+        <f t="shared" ref="I20" si="20">(1-(I19/I18))*100</f>
+        <v>96.894409937888199</v>
+      </c>
+      <c r="J20" s="22">
+        <f>(1-(J19/J18))*100</f>
+        <v>24.536256323777394</v>
+      </c>
+      <c r="K20" s="22">
+        <f>(1-(K19/K18))*100</f>
+        <v>65.420560747663558</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="10">
+        <v>7</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C21" s="33">
+        <v>25</v>
+      </c>
+      <c r="D21" s="33">
+        <v>75</v>
+      </c>
+      <c r="E21" s="33">
+        <v>9.5</v>
+      </c>
+      <c r="F21" s="8"/>
+      <c r="G21" s="8"/>
+      <c r="H21" s="8"/>
+      <c r="I21" s="8"/>
+      <c r="J21" s="8"/>
+      <c r="K21" s="8"/>
+    </row>
+    <row r="22" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="10">
+        <v>7</v>
+      </c>
+      <c r="B22" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C22" s="33">
+        <v>25</v>
+      </c>
+      <c r="D22" s="33">
+        <v>75</v>
+      </c>
+      <c r="E22" s="33">
+        <v>9.5</v>
+      </c>
+      <c r="F22" s="8"/>
+      <c r="G22" s="8"/>
+      <c r="H22" s="8"/>
+      <c r="I22" s="8"/>
+      <c r="J22" s="8"/>
+      <c r="K22" s="8"/>
+    </row>
+    <row r="23" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="10">
+        <v>7</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C23" s="33">
+        <v>25</v>
+      </c>
+      <c r="D23" s="33">
+        <v>75</v>
+      </c>
+      <c r="E23" s="33">
+        <v>9.5</v>
+      </c>
+      <c r="F23" s="8" t="e">
+        <f t="shared" ref="F23" si="21">(1-(F22/F21))*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G23" s="8" t="e">
+        <f t="shared" ref="G23" si="22">(1-(G22/G21))*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H23" s="8" t="e">
+        <f t="shared" ref="H23" si="23">(1-(H22/H21))*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I23" s="8" t="e">
+        <f t="shared" ref="I23" si="24">(1-(I22/I21))*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J23" s="8" t="e">
+        <f>(1-(J22/J21))*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K23" s="8" t="e">
+        <f>(1-(K22/K21))*100</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="11">
+        <v>8</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C24" s="32">
+        <v>50</v>
+      </c>
+      <c r="D24" s="32">
+        <v>75</v>
+      </c>
+      <c r="E24" s="32">
+        <v>9.5</v>
+      </c>
+      <c r="F24" s="22">
+        <v>2.8</v>
+      </c>
+      <c r="G24" s="22">
+        <v>265</v>
+      </c>
+      <c r="H24" s="22">
+        <v>76</v>
+      </c>
+      <c r="I24" s="22">
+        <v>553</v>
+      </c>
+      <c r="J24" s="22">
+        <v>67.599999999999994</v>
+      </c>
+      <c r="K24" s="22">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="11">
+        <v>8</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C25" s="32">
+        <v>50</v>
+      </c>
+      <c r="D25" s="32">
+        <v>75</v>
+      </c>
+      <c r="E25" s="32">
+        <v>9.5</v>
+      </c>
+      <c r="F25" s="22">
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="G25" s="22">
+        <v>81</v>
+      </c>
+      <c r="H25" s="22">
+        <v>78</v>
+      </c>
+      <c r="I25" s="22">
+        <v>5</v>
+      </c>
+      <c r="J25" s="22">
+        <v>49.1</v>
+      </c>
+      <c r="K25" s="22">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="11">
+        <v>8</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C26" s="32">
+        <v>50</v>
+      </c>
+      <c r="D26" s="32">
+        <v>75</v>
+      </c>
+      <c r="E26" s="32">
+        <v>9.5</v>
+      </c>
+      <c r="F26" s="22">
+        <f t="shared" ref="F26" si="25">(1-(F25/F24))*100</f>
+        <v>58.571428571428577</v>
+      </c>
+      <c r="G26" s="22">
+        <f t="shared" ref="G26" si="26">(1-(G25/G24))*100</f>
+        <v>69.433962264150949</v>
+      </c>
+      <c r="H26" s="22">
+        <f t="shared" ref="H26" si="27">(1-(H25/H24))*100</f>
+        <v>-2.6315789473684292</v>
+      </c>
+      <c r="I26" s="22">
+        <f t="shared" ref="I26" si="28">(1-(I25/I24))*100</f>
+        <v>99.095840867992763</v>
+      </c>
+      <c r="J26" s="22">
+        <f>(1-(J25/J24))*100</f>
+        <v>27.366863905325435</v>
+      </c>
+      <c r="K26" s="22">
+        <f>(1-(K25/K24))*100</f>
+        <v>67.285382830626446</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="11">
+        <v>9</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C27" s="32">
+        <v>75</v>
+      </c>
+      <c r="D27" s="32">
+        <v>75</v>
+      </c>
+      <c r="E27" s="32">
+        <v>9.5</v>
+      </c>
+      <c r="F27" s="22">
+        <v>3.06</v>
+      </c>
+      <c r="G27" s="22">
+        <v>212</v>
+      </c>
+      <c r="H27" s="22">
+        <v>167</v>
+      </c>
+      <c r="I27" s="22">
+        <v>160</v>
+      </c>
+      <c r="J27" s="22">
+        <v>70.5</v>
+      </c>
+      <c r="K27" s="22">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="11">
+        <v>9</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C28" s="32">
+        <v>75</v>
+      </c>
+      <c r="D28" s="32">
+        <v>75</v>
+      </c>
+      <c r="E28" s="32">
+        <v>9.5</v>
+      </c>
+      <c r="F28" s="22">
+        <v>1.56</v>
+      </c>
+      <c r="G28" s="22">
+        <v>91</v>
+      </c>
+      <c r="H28" s="22">
+        <v>143</v>
+      </c>
+      <c r="I28" s="22">
+        <v>5</v>
+      </c>
+      <c r="J28" s="22">
+        <v>49.1</v>
+      </c>
+      <c r="K28" s="22">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="11">
+        <v>9</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C29" s="32">
+        <v>75</v>
+      </c>
+      <c r="D29" s="32">
+        <v>75</v>
+      </c>
+      <c r="E29" s="32">
+        <v>9.5</v>
+      </c>
+      <c r="F29" s="22">
+        <f t="shared" ref="F29" si="29">(1-(F28/F27))*100</f>
+        <v>49.019607843137258</v>
+      </c>
+      <c r="G29" s="22">
+        <f t="shared" ref="G29" si="30">(1-(G28/G27))*100</f>
+        <v>57.075471698113198</v>
+      </c>
+      <c r="H29" s="22">
+        <f t="shared" ref="H29" si="31">(1-(H28/H27))*100</f>
+        <v>14.371257485029943</v>
+      </c>
+      <c r="I29" s="22">
+        <f t="shared" ref="I29" si="32">(1-(I28/I27))*100</f>
+        <v>96.875</v>
+      </c>
+      <c r="J29" s="22">
+        <f>(1-(J28/J27))*100</f>
+        <v>30.354609929078013</v>
+      </c>
+      <c r="K29" s="22">
+        <f>(1-(K28/K27))*100</f>
+        <v>72.505543237250563</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="10">
+        <v>10</v>
+      </c>
+      <c r="B30" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C30" s="33">
+        <v>25</v>
+      </c>
+      <c r="D30" s="33">
+        <v>125</v>
+      </c>
+      <c r="E30" s="33">
+        <v>9.5</v>
+      </c>
+      <c r="F30" s="8"/>
+      <c r="G30" s="8"/>
+      <c r="H30" s="8"/>
+      <c r="I30" s="8"/>
+      <c r="J30" s="8"/>
+      <c r="K30" s="8"/>
+    </row>
+    <row r="31" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="10">
+        <v>10</v>
+      </c>
+      <c r="B31" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C31" s="33">
+        <v>25</v>
+      </c>
+      <c r="D31" s="33">
+        <v>125</v>
+      </c>
+      <c r="E31" s="33">
+        <v>9.5</v>
+      </c>
+      <c r="F31" s="8"/>
+      <c r="G31" s="8"/>
+      <c r="H31" s="8"/>
+      <c r="I31" s="8"/>
+      <c r="J31" s="8"/>
+      <c r="K31" s="8"/>
+    </row>
+    <row r="32" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="10">
+        <v>10</v>
+      </c>
+      <c r="B32" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C32" s="33">
+        <v>25</v>
+      </c>
+      <c r="D32" s="33">
+        <v>125</v>
+      </c>
+      <c r="E32" s="33">
+        <v>9.5</v>
+      </c>
+      <c r="F32" s="8" t="e">
+        <f t="shared" ref="F32" si="33">(1-(F31/F30))*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G32" s="8" t="e">
+        <f t="shared" ref="G32" si="34">(1-(G31/G30))*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H32" s="8" t="e">
+        <f t="shared" ref="H32" si="35">(1-(H31/H30))*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I32" s="8" t="e">
+        <f t="shared" ref="I32" si="36">(1-(I31/I30))*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J32" s="8" t="e">
+        <f>(1-(J31/J30))*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K32" s="8" t="e">
+        <f>(1-(K31/K30))*100</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="11">
+        <v>11</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C33" s="32">
+        <v>50</v>
+      </c>
+      <c r="D33" s="32">
+        <v>125</v>
+      </c>
+      <c r="E33" s="32">
+        <v>9.5</v>
+      </c>
+      <c r="F33" s="22"/>
+      <c r="G33" s="22"/>
+      <c r="H33" s="22"/>
+      <c r="I33" s="22"/>
+      <c r="J33" s="22">
+        <f>2*61.5</f>
+        <v>123</v>
+      </c>
+      <c r="K33" s="22"/>
+    </row>
+    <row r="34" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="11">
+        <v>11</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C34" s="32">
+        <v>50</v>
+      </c>
+      <c r="D34" s="32">
+        <v>125</v>
+      </c>
+      <c r="E34" s="32">
+        <v>9.5</v>
+      </c>
+      <c r="F34" s="22"/>
+      <c r="G34" s="22"/>
+      <c r="H34" s="22"/>
+      <c r="I34" s="22"/>
+      <c r="J34" s="22">
+        <f>86.3</f>
+        <v>86.3</v>
+      </c>
+      <c r="K34" s="22"/>
+    </row>
+    <row r="35" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="11">
+        <v>11</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C35" s="32">
+        <v>50</v>
+      </c>
+      <c r="D35" s="32">
+        <v>125</v>
+      </c>
+      <c r="E35" s="32">
+        <v>9.5</v>
+      </c>
+      <c r="F35" s="22" t="e">
+        <f t="shared" ref="F35" si="37">(1-(F34/F33))*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G35" s="22" t="e">
+        <f t="shared" ref="G35" si="38">(1-(G34/G33))*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H35" s="22" t="e">
+        <f t="shared" ref="H35" si="39">(1-(H34/H33))*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I35" s="22" t="e">
+        <f t="shared" ref="I35" si="40">(1-(I34/I33))*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J35" s="22">
+        <f>(1-(J34/J33))*100</f>
+        <v>29.837398373983739</v>
+      </c>
+      <c r="K35" s="22" t="e">
+        <f>(1-(K34/K33))*100</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="11">
+        <v>12</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C36" s="32">
+        <v>75</v>
+      </c>
+      <c r="D36" s="32">
+        <v>125</v>
+      </c>
+      <c r="E36" s="32">
+        <v>9.5</v>
+      </c>
+      <c r="F36" s="22">
+        <v>1.98</v>
+      </c>
+      <c r="G36" s="22">
+        <v>212</v>
+      </c>
+      <c r="H36" s="22">
+        <v>163</v>
+      </c>
+      <c r="I36" s="22">
+        <v>153</v>
+      </c>
+      <c r="J36" s="22">
+        <f>2*59.3</f>
+        <v>118.6</v>
+      </c>
+      <c r="K36" s="22">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="11">
+        <v>12</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C37" s="32">
+        <v>75</v>
+      </c>
+      <c r="D37" s="32">
+        <v>125</v>
+      </c>
+      <c r="E37" s="32">
+        <v>9.5</v>
+      </c>
+      <c r="F37" s="22">
+        <v>1.24</v>
+      </c>
+      <c r="G37" s="22">
+        <v>98</v>
+      </c>
+      <c r="H37" s="22">
+        <v>161</v>
+      </c>
+      <c r="I37" s="22">
+        <v>5</v>
+      </c>
+      <c r="J37" s="22">
+        <v>79.2</v>
+      </c>
+      <c r="K37" s="22">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="11">
+        <v>12</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C38" s="32">
+        <v>75</v>
+      </c>
+      <c r="D38" s="32">
+        <v>125</v>
+      </c>
+      <c r="E38" s="32">
+        <v>9.5</v>
+      </c>
+      <c r="F38" s="22">
+        <f t="shared" ref="F38" si="41">(1-(F37/F36))*100</f>
+        <v>37.37373737373737</v>
+      </c>
+      <c r="G38" s="22">
+        <f t="shared" ref="G38" si="42">(1-(G37/G36))*100</f>
+        <v>53.773584905660378</v>
+      </c>
+      <c r="H38" s="22">
+        <f t="shared" ref="H38" si="43">(1-(H37/H36))*100</f>
+        <v>1.2269938650306789</v>
+      </c>
+      <c r="I38" s="22">
+        <f t="shared" ref="I38" si="44">(1-(I37/I36))*100</f>
+        <v>96.732026143790847</v>
+      </c>
+      <c r="J38" s="22">
+        <f>(1-(J37/J36))*100</f>
+        <v>33.220910623946033</v>
+      </c>
+      <c r="K38" s="22">
+        <f>(1-(K37/K36))*100</f>
+        <v>49.392712550607285</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="10">
+        <v>13</v>
+      </c>
+      <c r="B39" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C39" s="33">
+        <v>25</v>
+      </c>
+      <c r="D39" s="33">
+        <v>75</v>
+      </c>
+      <c r="E39" s="33">
+        <v>9.75</v>
+      </c>
+      <c r="F39" s="8"/>
+      <c r="G39" s="8"/>
+      <c r="H39" s="8"/>
+      <c r="I39" s="8"/>
+      <c r="J39" s="8"/>
+      <c r="K39" s="8"/>
+    </row>
+    <row r="40" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="10">
+        <v>13</v>
+      </c>
+      <c r="B40" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C40" s="33">
+        <v>25</v>
+      </c>
+      <c r="D40" s="33">
+        <v>75</v>
+      </c>
+      <c r="E40" s="33">
+        <v>9.75</v>
+      </c>
+      <c r="F40" s="8"/>
+      <c r="G40" s="8"/>
+      <c r="H40" s="8"/>
+      <c r="I40" s="8"/>
+      <c r="J40" s="8"/>
+      <c r="K40" s="8"/>
+    </row>
+    <row r="41" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="10">
+        <v>13</v>
+      </c>
+      <c r="B41" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C41" s="33">
+        <v>25</v>
+      </c>
+      <c r="D41" s="33">
+        <v>75</v>
+      </c>
+      <c r="E41" s="33">
+        <v>9.75</v>
+      </c>
+      <c r="F41" s="8" t="e">
+        <f t="shared" ref="F41" si="45">(1-(F40/F39))*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G41" s="8" t="e">
+        <f t="shared" ref="G41" si="46">(1-(G40/G39))*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H41" s="8" t="e">
+        <f t="shared" ref="H41" si="47">(1-(H40/H39))*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I41" s="8" t="e">
+        <f t="shared" ref="I41" si="48">(1-(I40/I39))*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J41" s="8" t="e">
+        <f>(1-(J40/J39))*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K41" s="8" t="e">
+        <f>(1-(K40/K39))*100</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="11">
+        <v>14</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C42" s="32">
+        <v>50</v>
+      </c>
+      <c r="D42" s="32">
+        <v>75</v>
+      </c>
+      <c r="E42" s="32">
+        <v>9.75</v>
+      </c>
+      <c r="F42" s="22">
+        <v>2.0699999999999998</v>
+      </c>
+      <c r="G42" s="22">
+        <v>288</v>
+      </c>
+      <c r="H42" s="22">
+        <v>168</v>
+      </c>
+      <c r="I42" s="22">
+        <v>460</v>
+      </c>
+      <c r="J42" s="22">
+        <v>69.900000000000006</v>
+      </c>
+      <c r="K42" s="22">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="11">
+        <v>14</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C43" s="32">
+        <v>50</v>
+      </c>
+      <c r="D43" s="32">
+        <v>75</v>
+      </c>
+      <c r="E43" s="32">
+        <v>9.75</v>
+      </c>
+      <c r="F43" s="22">
+        <v>1.03</v>
+      </c>
+      <c r="G43" s="22">
+        <v>101</v>
+      </c>
+      <c r="H43" s="22">
+        <v>156</v>
+      </c>
+      <c r="I43" s="22">
+        <v>5</v>
+      </c>
+      <c r="J43" s="22">
+        <v>44.9</v>
+      </c>
+      <c r="K43" s="22">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="11">
+        <v>14</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C44" s="32">
+        <v>50</v>
+      </c>
+      <c r="D44" s="32">
+        <v>75</v>
+      </c>
+      <c r="E44" s="32">
+        <v>9.75</v>
+      </c>
+      <c r="F44" s="22">
+        <f t="shared" ref="F44" si="49">(1-(F43/F42))*100</f>
+        <v>50.24154589371981</v>
+      </c>
+      <c r="G44" s="22">
+        <f t="shared" ref="G44" si="50">(1-(G43/G42))*100</f>
+        <v>64.930555555555557</v>
+      </c>
+      <c r="H44" s="22">
+        <f t="shared" ref="H44" si="51">(1-(H43/H42))*100</f>
+        <v>7.1428571428571397</v>
+      </c>
+      <c r="I44" s="22">
+        <f t="shared" ref="I44" si="52">(1-(I43/I42))*100</f>
+        <v>98.91304347826086</v>
+      </c>
+      <c r="J44" s="22">
+        <f>(1-(J43/J42))*100</f>
+        <v>35.765379113018604</v>
+      </c>
+      <c r="K44" s="22">
+        <f>(1-(K43/K42))*100</f>
+        <v>72.055427251732112</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="11">
+        <v>15</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C45" s="32">
+        <v>75</v>
+      </c>
+      <c r="D45" s="32">
+        <v>75</v>
+      </c>
+      <c r="E45" s="32">
+        <v>9.75</v>
+      </c>
+      <c r="F45" s="22">
+        <v>1.7</v>
+      </c>
+      <c r="G45" s="22">
+        <v>226</v>
+      </c>
+      <c r="H45" s="22">
+        <v>167</v>
+      </c>
+      <c r="I45" s="22">
+        <v>234</v>
+      </c>
+      <c r="J45" s="22">
+        <v>69.2</v>
+      </c>
+      <c r="K45" s="22">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="11">
+        <v>15</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C46" s="32">
+        <v>75</v>
+      </c>
+      <c r="D46" s="32">
+        <v>75</v>
+      </c>
+      <c r="E46" s="32">
+        <v>9.75</v>
+      </c>
+      <c r="F46" s="22">
+        <v>0.6</v>
+      </c>
+      <c r="G46" s="22">
+        <v>94</v>
+      </c>
+      <c r="H46" s="22">
+        <v>138</v>
+      </c>
+      <c r="I46" s="22">
+        <v>5</v>
+      </c>
+      <c r="J46" s="22">
+        <v>43.4</v>
+      </c>
+      <c r="K46" s="22">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="11">
+        <v>15</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C47" s="32">
+        <v>75</v>
+      </c>
+      <c r="D47" s="32">
+        <v>75</v>
+      </c>
+      <c r="E47" s="32">
+        <v>9.75</v>
+      </c>
+      <c r="F47" s="22">
+        <f t="shared" ref="F47" si="53">(1-(F46/F45))*100</f>
+        <v>64.705882352941174</v>
+      </c>
+      <c r="G47" s="22">
+        <f t="shared" ref="G47" si="54">(1-(G46/G45))*100</f>
+        <v>58.407079646017699</v>
+      </c>
+      <c r="H47" s="22">
+        <f t="shared" ref="H47" si="55">(1-(H46/H45))*100</f>
+        <v>17.365269461077848</v>
+      </c>
+      <c r="I47" s="22">
+        <f t="shared" ref="I47" si="56">(1-(I46/I45))*100</f>
+        <v>97.863247863247864</v>
+      </c>
+      <c r="J47" s="22">
+        <f>(1-(J46/J45))*100</f>
+        <v>37.283236994219656</v>
+      </c>
+      <c r="K47" s="22">
+        <f>(1-(K46/K45))*100</f>
+        <v>72.857142857142861</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="10">
+        <v>16</v>
+      </c>
+      <c r="B48" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C48" s="33">
+        <v>25</v>
+      </c>
+      <c r="D48" s="33">
+        <v>125</v>
+      </c>
+      <c r="E48" s="33">
+        <v>9.75</v>
+      </c>
+      <c r="F48" s="8"/>
+      <c r="G48" s="8"/>
+      <c r="H48" s="8"/>
+      <c r="I48" s="8"/>
+      <c r="J48" s="8"/>
+      <c r="K48" s="8"/>
+    </row>
+    <row r="49" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="10">
+        <v>16</v>
+      </c>
+      <c r="B49" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C49" s="33">
+        <v>25</v>
+      </c>
+      <c r="D49" s="33">
+        <v>125</v>
+      </c>
+      <c r="E49" s="33">
+        <v>9.75</v>
+      </c>
+      <c r="F49" s="8"/>
+      <c r="G49" s="8"/>
+      <c r="H49" s="8"/>
+      <c r="I49" s="8"/>
+      <c r="J49" s="8"/>
+      <c r="K49" s="8"/>
+    </row>
+    <row r="50" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="10">
+        <v>16</v>
+      </c>
+      <c r="B50" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C50" s="33">
+        <v>25</v>
+      </c>
+      <c r="D50" s="33">
+        <v>125</v>
+      </c>
+      <c r="E50" s="33">
+        <v>9.75</v>
+      </c>
+      <c r="F50" s="8" t="e">
+        <f t="shared" ref="F50" si="57">(1-(F49/F48))*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G50" s="8" t="e">
+        <f t="shared" ref="G50" si="58">(1-(G49/G48))*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H50" s="8" t="e">
+        <f t="shared" ref="H50" si="59">(1-(H49/H48))*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I50" s="8" t="e">
+        <f t="shared" ref="I50" si="60">(1-(I49/I48))*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J50" s="8" t="e">
+        <f>(1-(J49/J48))*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K50" s="8" t="e">
+        <f>(1-(K49/K48))*100</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="11">
+        <v>17</v>
+      </c>
+      <c r="B51" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C51" s="32">
+        <v>50</v>
+      </c>
+      <c r="D51" s="32">
+        <v>125</v>
+      </c>
+      <c r="E51" s="32">
+        <v>9.75</v>
+      </c>
+      <c r="F51" s="22"/>
+      <c r="G51" s="22"/>
+      <c r="H51" s="22"/>
+      <c r="I51" s="22"/>
+      <c r="J51" s="22">
+        <f>2*61.1</f>
+        <v>122.2</v>
+      </c>
+      <c r="K51" s="22"/>
+    </row>
+    <row r="52" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="11">
+        <v>17</v>
+      </c>
+      <c r="B52" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C52" s="32">
+        <v>50</v>
+      </c>
+      <c r="D52" s="32">
+        <v>125</v>
+      </c>
+      <c r="E52" s="32">
+        <v>9.75</v>
+      </c>
+      <c r="F52" s="22"/>
+      <c r="G52" s="22"/>
+      <c r="H52" s="22"/>
+      <c r="I52" s="22"/>
+      <c r="J52" s="22">
+        <v>76.7</v>
+      </c>
+      <c r="K52" s="22"/>
+    </row>
+    <row r="53" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="11">
+        <v>17</v>
+      </c>
+      <c r="B53" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C53" s="32">
+        <v>50</v>
+      </c>
+      <c r="D53" s="32">
+        <v>125</v>
+      </c>
+      <c r="E53" s="32">
+        <v>9.75</v>
+      </c>
+      <c r="F53" s="22" t="e">
+        <f t="shared" ref="F53" si="61">(1-(F52/F51))*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G53" s="22" t="e">
+        <f t="shared" ref="G53" si="62">(1-(G52/G51))*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H53" s="22" t="e">
+        <f t="shared" ref="H53" si="63">(1-(H52/H51))*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I53" s="22" t="e">
+        <f t="shared" ref="I53" si="64">(1-(I52/I51))*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J53" s="22">
+        <f>(1-(J52/J51))*100</f>
+        <v>37.234042553191493</v>
+      </c>
+      <c r="K53" s="22" t="e">
+        <f>(1-(K52/K51))*100</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="11">
+        <v>18</v>
+      </c>
+      <c r="B54" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C54" s="32">
+        <v>75</v>
+      </c>
+      <c r="D54" s="32">
+        <v>125</v>
+      </c>
+      <c r="E54" s="32">
+        <v>9.75</v>
+      </c>
+      <c r="F54" s="22">
+        <v>1.7</v>
+      </c>
+      <c r="G54" s="22">
+        <v>231</v>
+      </c>
+      <c r="H54" s="22">
+        <v>184</v>
+      </c>
+      <c r="I54" s="22">
+        <v>157</v>
+      </c>
+      <c r="J54" s="22">
+        <f>2*59</f>
+        <v>118</v>
+      </c>
+      <c r="K54" s="22">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="11">
+        <v>18</v>
+      </c>
+      <c r="B55" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C55" s="32">
+        <v>75</v>
+      </c>
+      <c r="D55" s="32">
+        <v>125</v>
+      </c>
+      <c r="E55" s="32">
+        <v>9.75</v>
+      </c>
+      <c r="F55" s="22">
+        <v>0.93</v>
+      </c>
+      <c r="G55" s="22">
+        <v>94</v>
+      </c>
+      <c r="H55" s="22">
+        <v>150</v>
+      </c>
+      <c r="I55" s="22">
+        <v>5</v>
+      </c>
+      <c r="J55" s="22">
+        <v>66.5</v>
+      </c>
+      <c r="K55" s="22">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="11">
+        <v>18</v>
+      </c>
+      <c r="B56" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C56" s="32">
+        <v>75</v>
+      </c>
+      <c r="D56" s="32">
+        <v>125</v>
+      </c>
+      <c r="E56" s="32">
+        <v>9.75</v>
+      </c>
+      <c r="F56" s="22">
+        <f t="shared" ref="F56" si="65">(1-(F55/F54))*100</f>
+        <v>45.294117647058819</v>
+      </c>
+      <c r="G56" s="22">
+        <f t="shared" ref="G56" si="66">(1-(G55/G54))*100</f>
+        <v>59.307359307359306</v>
+      </c>
+      <c r="H56" s="22">
+        <f t="shared" ref="H56" si="67">(1-(H55/H54))*100</f>
+        <v>18.478260869565222</v>
+      </c>
+      <c r="I56" s="22">
+        <f t="shared" ref="I56" si="68">(1-(I55/I54))*100</f>
+        <v>96.815286624203821</v>
+      </c>
+      <c r="J56" s="22">
+        <f>(1-(J55/J54))*100</f>
+        <v>43.644067796610166</v>
+      </c>
+      <c r="K56" s="22">
+        <f>(1-(K55/K54))*100</f>
+        <v>75.813953488372093</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67DE9CC2-1390-4757-88D3-4EDA69644CAD}">
   <dimension ref="A3:CH27"/>
   <sheetViews>
@@ -2612,6 +4525,7 @@
       <selection activeCell="F26" sqref="F26"/>
     </sheetView>
     <sheetView workbookViewId="2"/>
+    <sheetView workbookViewId="3"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2619,18 +4533,18 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:86" x14ac:dyDescent="0.25">
-      <c r="C3" s="26" t="s">
+      <c r="C3" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="26"/>
-      <c r="E3" s="26"/>
-      <c r="F3" s="26"/>
-      <c r="G3" s="26" t="s">
+      <c r="D3" s="34"/>
+      <c r="E3" s="34"/>
+      <c r="F3" s="34"/>
+      <c r="G3" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="26"/>
-      <c r="I3" s="26"/>
-      <c r="J3" s="26"/>
+      <c r="H3" s="34"/>
+      <c r="I3" s="34"/>
+      <c r="J3" s="34"/>
     </row>
     <row r="4" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -3868,6 +5782,79 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_dlc_DocId xmlns="add409d8-c458-45bf-bf5f-710f0ed12ba3">CY54R7KD54KC-91199970-192712</_dlc_DocId>
+    <DLCPolicyLabelLock xmlns="B9FBF822-0A65-4D1F-BC13-C27C7257EFA0" xsi:nil="true"/>
+    <DLCPolicyLabelClientValue xmlns="B9FBF822-0A65-4D1F-BC13-C27C7257EFA0" xsi:nil="true"/>
+    <_dlc_DocIdUrl xmlns="add409d8-c458-45bf-bf5f-710f0ed12ba3">
+      <Url>https://grundfos.sharepoint.com/sites/Pro-017826/_layouts/15/DocIdRedir.aspx?ID=CY54R7KD54KC-91199970-192712</Url>
+      <Description>CY54R7KD54KC-91199970-192712</Description>
+    </_dlc_DocIdUrl>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10001</Type>
+    <SequenceNumber>1000</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10002</Type>
+    <SequenceNumber>1001</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10004</Type>
+    <SequenceNumber>1002</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10006</Type>
+    <SequenceNumber>1003</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+</spe:Receivers>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010013E660C0EEA2F44AA3B088C58E7762CB" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="5484fa9f9b42a97565e65fac7903a307">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="add409d8-c458-45bf-bf5f-710f0ed12ba3" xmlns:ns3="B9FBF822-0A65-4D1F-BC13-C27C7257EFA0" xmlns:ns4="b9fbf822-0a65-4d1f-bc13-c27c7257efa0" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="de45a4d41d0ddc6d7e8e18579ff54800" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="add409d8-c458-45bf-bf5f-710f0ed12ba3"/>
@@ -4134,80 +6121,34 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10001</Type>
-    <SequenceNumber>1000</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10002</Type>
-    <SequenceNumber>1001</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10004</Type>
-    <SequenceNumber>1002</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10006</Type>
-    <SequenceNumber>1003</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-</spe:Receivers>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F80D695E-02F0-4FF4-A9B6-96C7E8E5A419}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="add409d8-c458-45bf-bf5f-710f0ed12ba3"/>
+    <ds:schemaRef ds:uri="B9FBF822-0A65-4D1F-BC13-C27C7257EFA0"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{51CC3469-56E6-4BF6-AD20-3A6F9B943A35}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_dlc_DocId xmlns="add409d8-c458-45bf-bf5f-710f0ed12ba3">CY54R7KD54KC-91199970-192712</_dlc_DocId>
-    <DLCPolicyLabelLock xmlns="B9FBF822-0A65-4D1F-BC13-C27C7257EFA0" xsi:nil="true"/>
-    <DLCPolicyLabelClientValue xmlns="B9FBF822-0A65-4D1F-BC13-C27C7257EFA0" xsi:nil="true"/>
-    <_dlc_DocIdUrl xmlns="add409d8-c458-45bf-bf5f-710f0ed12ba3">
-      <Url>https://grundfos.sharepoint.com/sites/Pro-017826/_layouts/15/DocIdRedir.aspx?ID=CY54R7KD54KC-91199970-192712</Url>
-      <Description>CY54R7KD54KC-91199970-192712</Description>
-    </_dlc_DocIdUrl>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D23B5ADC-2FED-4856-AE1D-6D8A5A36E916}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E0D66368-F85C-4561-B8C5-570B6192D2BA}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4225,31 +6166,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D23B5ADC-2FED-4856-AE1D-6D8A5A36E916}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{51CC3469-56E6-4BF6-AD20-3A6F9B943A35}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F80D695E-02F0-4FF4-A9B6-96C7E8E5A419}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="add409d8-c458-45bf-bf5f-710f0ed12ba3"/>
-    <ds:schemaRef ds:uri="B9FBF822-0A65-4D1F-BC13-C27C7257EFA0"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
gennemgang af modellos :)
</commit_message>
<xml_diff>
--- a/data/SPRR/SPRR_analysesvar_samlet.xlsx
+++ b/data/SPRR/SPRR_analysesvar_samlet.xlsx
@@ -5,15 +5,15 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://grundfos-my.sharepoint.com/personal/102222_grundfos_com/Documents/Desktop/Speciale/data/SPRR/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://grundfos-my.sharepoint.com/personal/103195_grundfos_com/Documents/Code/Speciale/data/SPRR/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="484" documentId="8_{B1838E2C-57DF-442F-BA8D-29F29F483C5A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{B62C7BD0-2F0E-49B2-BE24-ADBDA4838062}"/>
+  <xr:revisionPtr revIDLastSave="485" documentId="8_{B1838E2C-57DF-442F-BA8D-29F29F483C5A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{7E94B02B-0541-4E82-8DA5-9F7A3F5FEA06}"/>
   <bookViews>
-    <workbookView visibility="hidden" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4945AC14-70B2-4790-A402-2CEEE388F912}"/>
-    <workbookView visibility="hidden" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{F3BEDCAF-2F4D-48AD-8D56-F91ED459115A}"/>
-    <workbookView visibility="hidden" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B1D28580-2409-4DF1-802D-4DFBB9E40CE8}"/>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{2BA11759-6010-40F7-B40A-A3F9569E799B}"/>
+    <workbookView visibility="hidden" xWindow="2200" yWindow="2200" windowWidth="14400" windowHeight="7810" xr2:uid="{4945AC14-70B2-4790-A402-2CEEE388F912}"/>
+    <workbookView visibility="hidden" xWindow="2200" yWindow="2200" windowWidth="14400" windowHeight="7810" activeTab="1" xr2:uid="{F3BEDCAF-2F4D-48AD-8D56-F91ED459115A}"/>
+    <workbookView visibility="hidden" xWindow="2200" yWindow="2200" windowWidth="14400" windowHeight="7810" xr2:uid="{B1D28580-2409-4DF1-802D-4DFBB9E40CE8}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" activeTab="2" xr2:uid="{2BA11759-6010-40F7-B40A-A3F9569E799B}"/>
   </bookViews>
   <sheets>
     <sheet name="analyse svar" sheetId="2" r:id="rId1"/>
@@ -481,6 +481,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -494,15 +503,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -837,12 +837,12 @@
       <selection activeCell="C1" sqref="C1:E1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="11" max="11" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="C3" s="75" t="s">
         <v>9</v>
       </c>
@@ -852,7 +852,7 @@
       </c>
       <c r="F3" s="75"/>
     </row>
-    <row r="4" spans="1:14" ht="23.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" ht="23.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -896,7 +896,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:14" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A5" s="28">
         <v>1</v>
       </c>
@@ -936,7 +936,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="6" spans="1:14" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="28">
         <v>1</v>
       </c>
@@ -958,7 +958,7 @@
       <c r="M6" s="25"/>
       <c r="N6" s="25"/>
     </row>
-    <row r="7" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="11">
         <v>2</v>
       </c>
@@ -998,7 +998,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="8" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A8" s="11">
         <v>2</v>
       </c>
@@ -1020,7 +1020,7 @@
       <c r="M8" s="22"/>
       <c r="N8" s="22"/>
     </row>
-    <row r="9" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="11">
         <v>3</v>
       </c>
@@ -1060,7 +1060,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="10" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A10" s="11">
         <v>3</v>
       </c>
@@ -1082,7 +1082,7 @@
       <c r="M10" s="22"/>
       <c r="N10" s="22"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A11" s="10">
         <v>4</v>
       </c>
@@ -1120,7 +1120,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A12" s="10">
         <v>4</v>
       </c>
@@ -1140,7 +1140,7 @@
       <c r="M12" s="8"/>
       <c r="N12" s="8"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A13" s="11">
         <v>5</v>
       </c>
@@ -1191,7 +1191,7 @@
         <v>66.516853932584269</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A14" s="11">
         <v>5</v>
       </c>
@@ -1223,7 +1223,7 @@
       </c>
       <c r="N14" s="8"/>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A15" s="11">
         <v>6</v>
       </c>
@@ -1274,7 +1274,7 @@
         <v>65.420560747663558</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A16" s="11">
         <v>6</v>
       </c>
@@ -1307,7 +1307,7 @@
       </c>
       <c r="N16" s="8"/>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A17" s="10">
         <v>7</v>
       </c>
@@ -1345,7 +1345,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A18" s="10">
         <v>7</v>
       </c>
@@ -1365,7 +1365,7 @@
       <c r="M18" s="8"/>
       <c r="N18" s="8"/>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A19" s="11">
         <v>8</v>
       </c>
@@ -1415,7 +1415,7 @@
         <v>67.285382830626446</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A20" s="11">
         <v>8</v>
       </c>
@@ -1447,7 +1447,7 @@
       </c>
       <c r="N20" s="8"/>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A21" s="11">
         <v>9</v>
       </c>
@@ -1497,7 +1497,7 @@
         <v>72.505543237250563</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A22" s="11">
         <v>9</v>
       </c>
@@ -1529,7 +1529,7 @@
       </c>
       <c r="N22" s="8"/>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A23" s="10">
         <v>10</v>
       </c>
@@ -1567,7 +1567,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A24" s="10">
         <v>10</v>
       </c>
@@ -1587,7 +1587,7 @@
       <c r="M24" s="8"/>
       <c r="N24" s="8"/>
     </row>
-    <row r="25" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A25" s="11">
         <v>11</v>
       </c>
@@ -1628,7 +1628,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="26" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A26" s="11">
         <v>11</v>
       </c>
@@ -1651,7 +1651,7 @@
       <c r="M26" s="22"/>
       <c r="N26" s="22"/>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A27" s="11">
         <v>12</v>
       </c>
@@ -1702,7 +1702,7 @@
         <v>49.392712550607285</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A28" s="11">
         <v>12</v>
       </c>
@@ -1734,7 +1734,7 @@
       </c>
       <c r="N28" s="8"/>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A29" s="10">
         <v>13</v>
       </c>
@@ -1772,7 +1772,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A30" s="10">
         <v>13</v>
       </c>
@@ -1792,7 +1792,7 @@
       <c r="M30" s="8"/>
       <c r="N30" s="8"/>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A31" s="11">
         <v>14</v>
       </c>
@@ -1842,7 +1842,7 @@
         <v>72.055427251732112</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A32" s="11">
         <v>14</v>
       </c>
@@ -1874,7 +1874,7 @@
       </c>
       <c r="N32" s="8"/>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A33" s="11">
         <v>15</v>
       </c>
@@ -1924,7 +1924,7 @@
         <v>72.857142857142861</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A34" s="11">
         <v>15</v>
       </c>
@@ -1956,7 +1956,7 @@
       </c>
       <c r="N34" s="8"/>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A35" s="10">
         <v>16</v>
       </c>
@@ -1994,7 +1994,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A36" s="10">
         <v>16</v>
       </c>
@@ -2014,7 +2014,7 @@
       <c r="M36" s="8"/>
       <c r="N36" s="8"/>
     </row>
-    <row r="37" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A37" s="11">
         <v>17</v>
       </c>
@@ -2055,7 +2055,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="38" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A38" s="11">
         <v>17</v>
       </c>
@@ -2077,7 +2077,7 @@
       <c r="M38" s="22"/>
       <c r="N38" s="22"/>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A39" s="11">
         <v>18</v>
       </c>
@@ -2128,7 +2128,7 @@
         <v>75.813953488372093</v>
       </c>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A40" s="11">
         <v>18</v>
       </c>
@@ -2160,7 +2160,7 @@
       </c>
       <c r="N40" s="8"/>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A41" s="3"/>
     </row>
   </sheetData>
@@ -2184,15 +2184,15 @@
     <sheetView workbookViewId="2"/>
     <sheetView workbookViewId="3"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="7" width="9.140625" style="3"/>
-    <col min="8" max="8" width="9.140625" style="24"/>
-    <col min="22" max="23" width="9.140625" style="3"/>
-    <col min="34" max="35" width="9.140625" style="3"/>
+    <col min="2" max="7" width="9.1796875" style="3"/>
+    <col min="8" max="8" width="9.1796875" style="24"/>
+    <col min="22" max="23" width="9.1796875" style="3"/>
+    <col min="34" max="35" width="9.1796875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:37" x14ac:dyDescent="0.35">
       <c r="B1" s="3">
         <v>1</v>
       </c>
@@ -2302,7 +2302,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -2415,7 +2415,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -2488,7 +2488,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="4" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -2561,7 +2561,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="5" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -2634,7 +2634,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="6" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>25</v>
       </c>
@@ -2707,7 +2707,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>23</v>
       </c>
@@ -2800,7 +2800,7 @@
         <v>66.5</v>
       </c>
     </row>
-    <row r="8" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>24</v>
       </c>
@@ -2873,7 +2873,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="9" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:37" x14ac:dyDescent="0.35">
       <c r="I9" s="24"/>
       <c r="N9" s="24"/>
       <c r="O9" s="24"/>
@@ -2896,17 +2896,17 @@
     <sheetView workbookViewId="0"/>
     <sheetView workbookViewId="1"/>
     <sheetView workbookViewId="2"/>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="3">
-      <selection activeCell="M54" sqref="M54"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="90" zoomScaleNormal="90" workbookViewId="3">
+      <selection activeCell="K53" sqref="K53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="F1" s="30"/>
       <c r="G1" s="30"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>33</v>
       </c>
@@ -2941,7 +2941,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:11" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="28">
         <v>1</v>
       </c>
@@ -2974,7 +2974,7 @@
       </c>
       <c r="K3" s="25"/>
     </row>
-    <row r="4" spans="1:11" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" s="28">
         <v>1</v>
       </c>
@@ -3007,7 +3007,7 @@
       </c>
       <c r="K4" s="25"/>
     </row>
-    <row r="5" spans="1:11" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A5" s="28">
         <v>1</v>
       </c>
@@ -3048,7 +3048,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="6" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="11">
         <v>2</v>
       </c>
@@ -3083,7 +3083,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="7" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="11">
         <v>2</v>
       </c>
@@ -3118,7 +3118,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="8" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A8" s="11">
         <v>2</v>
       </c>
@@ -3159,7 +3159,7 @@
         <v>61.29032258064516</v>
       </c>
     </row>
-    <row r="9" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="11">
         <v>3</v>
       </c>
@@ -3194,7 +3194,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="10" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A10" s="11">
         <v>3</v>
       </c>
@@ -3229,7 +3229,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="11" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A11" s="11">
         <v>3</v>
       </c>
@@ -3270,7 +3270,7 @@
         <v>65.934065934065927</v>
       </c>
     </row>
-    <row r="12" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A12" s="10">
         <v>4</v>
       </c>
@@ -3293,7 +3293,7 @@
       <c r="J12" s="8"/>
       <c r="K12" s="8"/>
     </row>
-    <row r="13" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A13" s="10">
         <v>4</v>
       </c>
@@ -3316,7 +3316,7 @@
       <c r="J13" s="8"/>
       <c r="K13" s="8"/>
     </row>
-    <row r="14" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A14" s="10">
         <v>4</v>
       </c>
@@ -3357,7 +3357,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="15" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A15" s="11">
         <v>5</v>
       </c>
@@ -3393,7 +3393,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="16" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A16" s="11">
         <v>5</v>
       </c>
@@ -3428,7 +3428,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="17" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A17" s="11">
         <v>5</v>
       </c>
@@ -3469,7 +3469,7 @@
         <v>66.516853932584269</v>
       </c>
     </row>
-    <row r="18" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A18" s="11">
         <v>6</v>
       </c>
@@ -3505,7 +3505,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="19" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A19" s="11">
         <v>6</v>
       </c>
@@ -3541,7 +3541,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="20" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A20" s="11">
         <v>6</v>
       </c>
@@ -3582,7 +3582,7 @@
         <v>65.420560747663558</v>
       </c>
     </row>
-    <row r="21" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A21" s="10">
         <v>7</v>
       </c>
@@ -3605,7 +3605,7 @@
       <c r="J21" s="8"/>
       <c r="K21" s="8"/>
     </row>
-    <row r="22" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A22" s="10">
         <v>7</v>
       </c>
@@ -3628,7 +3628,7 @@
       <c r="J22" s="8"/>
       <c r="K22" s="8"/>
     </row>
-    <row r="23" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A23" s="10">
         <v>7</v>
       </c>
@@ -3669,7 +3669,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="24" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A24" s="11">
         <v>8</v>
       </c>
@@ -3704,7 +3704,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="25" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A25" s="11">
         <v>8</v>
       </c>
@@ -3739,7 +3739,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="26" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A26" s="11">
         <v>8</v>
       </c>
@@ -3780,7 +3780,7 @@
         <v>67.285382830626446</v>
       </c>
     </row>
-    <row r="27" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A27" s="11">
         <v>9</v>
       </c>
@@ -3815,7 +3815,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="28" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A28" s="11">
         <v>9</v>
       </c>
@@ -3850,7 +3850,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="29" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A29" s="11">
         <v>9</v>
       </c>
@@ -3891,7 +3891,7 @@
         <v>72.505543237250563</v>
       </c>
     </row>
-    <row r="30" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A30" s="10">
         <v>10</v>
       </c>
@@ -3914,7 +3914,7 @@
       <c r="J30" s="8"/>
       <c r="K30" s="8"/>
     </row>
-    <row r="31" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A31" s="10">
         <v>10</v>
       </c>
@@ -3937,7 +3937,7 @@
       <c r="J31" s="8"/>
       <c r="K31" s="8"/>
     </row>
-    <row r="32" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A32" s="10">
         <v>10</v>
       </c>
@@ -3978,7 +3978,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="33" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A33" s="11">
         <v>11</v>
       </c>
@@ -4014,7 +4014,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="34" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A34" s="11">
         <v>11</v>
       </c>
@@ -4050,7 +4050,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="35" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A35" s="11">
         <v>11</v>
       </c>
@@ -4091,7 +4091,7 @@
         <v>-6.0606060606060552</v>
       </c>
     </row>
-    <row r="36" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A36" s="11">
         <v>12</v>
       </c>
@@ -4127,7 +4127,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="37" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A37" s="11">
         <v>12</v>
       </c>
@@ -4162,7 +4162,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="38" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A38" s="11">
         <v>12</v>
       </c>
@@ -4203,7 +4203,7 @@
         <v>49.392712550607285</v>
       </c>
     </row>
-    <row r="39" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A39" s="10">
         <v>13</v>
       </c>
@@ -4226,7 +4226,7 @@
       <c r="J39" s="8"/>
       <c r="K39" s="8"/>
     </row>
-    <row r="40" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A40" s="10">
         <v>13</v>
       </c>
@@ -4249,7 +4249,7 @@
       <c r="J40" s="8"/>
       <c r="K40" s="8"/>
     </row>
-    <row r="41" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A41" s="10">
         <v>13</v>
       </c>
@@ -4290,7 +4290,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="42" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A42" s="11">
         <v>14</v>
       </c>
@@ -4325,7 +4325,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="43" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A43" s="11">
         <v>14</v>
       </c>
@@ -4360,7 +4360,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="44" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A44" s="11">
         <v>14</v>
       </c>
@@ -4401,7 +4401,7 @@
         <v>72.055427251732112</v>
       </c>
     </row>
-    <row r="45" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A45" s="11">
         <v>15</v>
       </c>
@@ -4436,7 +4436,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="46" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A46" s="11">
         <v>15</v>
       </c>
@@ -4471,7 +4471,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="47" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A47" s="11">
         <v>15</v>
       </c>
@@ -4512,7 +4512,7 @@
         <v>72.857142857142861</v>
       </c>
     </row>
-    <row r="48" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A48" s="10">
         <v>16</v>
       </c>
@@ -4535,7 +4535,7 @@
       <c r="J48" s="8"/>
       <c r="K48" s="8"/>
     </row>
-    <row r="49" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A49" s="10">
         <v>16</v>
       </c>
@@ -4558,7 +4558,7 @@
       <c r="J49" s="8"/>
       <c r="K49" s="8"/>
     </row>
-    <row r="50" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A50" s="10">
         <v>16</v>
       </c>
@@ -4599,7 +4599,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="51" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A51" s="11">
         <v>17</v>
       </c>
@@ -4631,9 +4631,11 @@
         <f>2*61.1</f>
         <v>122.2</v>
       </c>
-      <c r="K51" s="22"/>
-    </row>
-    <row r="52" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K51" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A52" s="11">
         <v>17</v>
       </c>
@@ -4668,7 +4670,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="53" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A53" s="11">
         <v>17</v>
       </c>
@@ -4709,7 +4711,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="54" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A54" s="11">
         <v>18</v>
       </c>
@@ -4745,7 +4747,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="55" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A55" s="11">
         <v>18</v>
       </c>
@@ -4780,7 +4782,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="56" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A56" s="11">
         <v>18</v>
       </c>
@@ -4833,21 +4835,21 @@
     <sheetView workbookViewId="0"/>
     <sheetView workbookViewId="1"/>
     <sheetView workbookViewId="2"/>
-    <sheetView tabSelected="1" topLeftCell="E24" zoomScaleNormal="100" workbookViewId="3">
+    <sheetView topLeftCell="E24" zoomScaleNormal="100" workbookViewId="3">
       <selection activeCell="P59" sqref="P59"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="12" max="12" width="8.85546875" style="37"/>
-    <col min="13" max="16" width="8.85546875" style="38"/>
-    <col min="17" max="17" width="8.85546875" style="39"/>
-    <col min="27" max="27" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.81640625" style="37"/>
+    <col min="13" max="16" width="8.81640625" style="38"/>
+    <col min="17" max="17" width="8.81640625" style="39"/>
+    <col min="27" max="27" width="13.7265625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="17.1796875" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.35">
       <c r="F1" s="75" t="s">
         <v>36</v>
       </c>
@@ -4856,22 +4858,22 @@
       <c r="I1" s="75"/>
       <c r="J1" s="75"/>
       <c r="K1" s="75"/>
-      <c r="L1" s="76" t="s">
+      <c r="L1" s="79" t="s">
         <v>39</v>
       </c>
-      <c r="M1" s="77"/>
-      <c r="N1" s="77"/>
-      <c r="O1" s="77"/>
-      <c r="P1" s="77"/>
-      <c r="Q1" s="78"/>
-      <c r="R1" s="76" t="s">
+      <c r="M1" s="80"/>
+      <c r="N1" s="80"/>
+      <c r="O1" s="80"/>
+      <c r="P1" s="80"/>
+      <c r="Q1" s="81"/>
+      <c r="R1" s="79" t="s">
         <v>40</v>
       </c>
-      <c r="S1" s="77"/>
-      <c r="T1" s="77"/>
-      <c r="U1" s="77"/>
-      <c r="V1" s="77"/>
-      <c r="W1" s="77"/>
+      <c r="S1" s="80"/>
+      <c r="T1" s="80"/>
+      <c r="U1" s="80"/>
+      <c r="V1" s="80"/>
+      <c r="W1" s="80"/>
       <c r="X1" s="47"/>
       <c r="Y1" s="48"/>
       <c r="Z1" s="48"/>
@@ -4879,7 +4881,7 @@
       <c r="AB1" s="48"/>
       <c r="AC1" s="49"/>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.35">
       <c r="E2" t="s">
         <v>38</v>
       </c>
@@ -4914,7 +4916,7 @@
       <c r="AB2" s="38"/>
       <c r="AC2" s="39"/>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.35">
       <c r="E3" t="s">
         <v>37</v>
       </c>
@@ -4936,16 +4938,16 @@
       <c r="K3">
         <v>1</v>
       </c>
-      <c r="R3" s="79" t="s">
+      <c r="R3" s="82" t="s">
         <v>41</v>
       </c>
-      <c r="S3" s="80"/>
-      <c r="T3" s="80" t="s">
+      <c r="S3" s="83"/>
+      <c r="T3" s="83" t="s">
         <v>42</v>
       </c>
-      <c r="U3" s="80"/>
-      <c r="V3" s="80"/>
-      <c r="W3" s="80"/>
+      <c r="U3" s="83"/>
+      <c r="V3" s="83"/>
+      <c r="W3" s="83"/>
       <c r="X3" s="37" t="s">
         <v>43</v>
       </c>
@@ -4955,13 +4957,13 @@
       <c r="Z3" s="38" t="s">
         <v>44</v>
       </c>
-      <c r="AA3" s="81" t="s">
+      <c r="AA3" s="76" t="s">
         <v>46</v>
       </c>
-      <c r="AB3" s="82"/>
-      <c r="AC3" s="83"/>
-    </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AB3" s="77"/>
+      <c r="AC3" s="78"/>
+    </row>
+    <row r="4" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>33</v>
       </c>
@@ -5050,7 +5052,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:29" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:29" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A5" s="28">
         <v>1</v>
       </c>
@@ -5155,7 +5157,7 @@
         <v>17.804207406813433</v>
       </c>
     </row>
-    <row r="6" spans="1:29" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:29" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="28">
         <v>1</v>
       </c>
@@ -5260,7 +5262,7 @@
         <v>-9.3793845918251773</v>
       </c>
     </row>
-    <row r="7" spans="1:29" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:29" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="28">
         <v>1</v>
       </c>
@@ -5313,7 +5315,7 @@
       <c r="AB7" s="65"/>
       <c r="AC7" s="66"/>
     </row>
-    <row r="8" spans="1:29" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:29" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A8" s="11">
         <v>2</v>
       </c>
@@ -5420,7 +5422,7 @@
         <v>-12.051263446371225</v>
       </c>
     </row>
-    <row r="9" spans="1:29" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:29" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="11">
         <v>2</v>
       </c>
@@ -5527,7 +5529,7 @@
         <v>-12.405099490165714</v>
       </c>
     </row>
-    <row r="10" spans="1:29" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:29" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A10" s="11">
         <v>2</v>
       </c>
@@ -5580,7 +5582,7 @@
       <c r="AB10" s="68"/>
       <c r="AC10" s="69"/>
     </row>
-    <row r="11" spans="1:29" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:29" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A11" s="11">
         <v>3</v>
       </c>
@@ -5687,7 +5689,7 @@
         <v>-27.378955134717348</v>
       </c>
     </row>
-    <row r="12" spans="1:29" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:29" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A12" s="11">
         <v>3</v>
       </c>
@@ -5794,7 +5796,7 @@
         <v>-25.224692401507916</v>
       </c>
     </row>
-    <row r="13" spans="1:29" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:29" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A13" s="11">
         <v>3</v>
       </c>
@@ -5847,7 +5849,7 @@
       <c r="AB13" s="68"/>
       <c r="AC13" s="69"/>
     </row>
-    <row r="14" spans="1:29" s="63" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:29" s="63" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A14" s="56">
         <v>4</v>
       </c>
@@ -5882,7 +5884,7 @@
       <c r="AB14" s="71"/>
       <c r="AC14" s="70"/>
     </row>
-    <row r="15" spans="1:29" s="63" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:29" s="63" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A15" s="56">
         <v>4</v>
       </c>
@@ -5917,7 +5919,7 @@
       <c r="AB15" s="71"/>
       <c r="AC15" s="70"/>
     </row>
-    <row r="16" spans="1:29" s="63" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:29" s="63" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A16" s="56">
         <v>4</v>
       </c>
@@ -5952,7 +5954,7 @@
       <c r="AB16" s="71"/>
       <c r="AC16" s="70"/>
     </row>
-    <row r="17" spans="1:29" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:29" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A17" s="11">
         <v>5</v>
       </c>
@@ -6060,7 +6062,7 @@
         <v>16.53978942811445</v>
       </c>
     </row>
-    <row r="18" spans="1:29" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:29" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A18" s="11">
         <v>5</v>
       </c>
@@ -6167,7 +6169,7 @@
         <v>0.69503082188391252</v>
       </c>
     </row>
-    <row r="19" spans="1:29" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:29" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A19" s="11">
         <v>5</v>
       </c>
@@ -6220,7 +6222,7 @@
       <c r="AB19" s="68"/>
       <c r="AC19" s="69"/>
     </row>
-    <row r="20" spans="1:29" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:29" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A20" s="11">
         <v>6</v>
       </c>
@@ -6328,7 +6330,7 @@
         <v>-10.198037211386723</v>
       </c>
     </row>
-    <row r="21" spans="1:29" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:29" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A21" s="11">
         <v>6</v>
       </c>
@@ -6436,7 +6438,7 @@
         <v>-0.97420519236615377</v>
       </c>
     </row>
-    <row r="22" spans="1:29" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:29" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A22" s="11">
         <v>6</v>
       </c>
@@ -6489,7 +6491,7 @@
       <c r="AB22" s="68"/>
       <c r="AC22" s="69"/>
     </row>
-    <row r="23" spans="1:29" s="63" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:29" s="63" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A23" s="56">
         <v>7</v>
       </c>
@@ -6524,7 +6526,7 @@
       <c r="AB23" s="71"/>
       <c r="AC23" s="70"/>
     </row>
-    <row r="24" spans="1:29" s="63" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:29" s="63" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A24" s="56">
         <v>7</v>
       </c>
@@ -6559,7 +6561,7 @@
       <c r="AB24" s="71"/>
       <c r="AC24" s="70"/>
     </row>
-    <row r="25" spans="1:29" s="63" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:29" s="63" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A25" s="56">
         <v>7</v>
       </c>
@@ -6594,7 +6596,7 @@
       <c r="AB25" s="71"/>
       <c r="AC25" s="70"/>
     </row>
-    <row r="26" spans="1:29" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:29" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A26" s="11">
         <v>8</v>
       </c>
@@ -6701,7 +6703,7 @@
         <v>17.019656945953081</v>
       </c>
     </row>
-    <row r="27" spans="1:29" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:29" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A27" s="11">
         <v>8</v>
       </c>
@@ -6808,7 +6810,7 @@
         <v>-35.808145860538168</v>
       </c>
     </row>
-    <row r="28" spans="1:29" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:29" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A28" s="11">
         <v>8</v>
       </c>
@@ -6861,7 +6863,7 @@
       <c r="AB28" s="68"/>
       <c r="AC28" s="69"/>
     </row>
-    <row r="29" spans="1:29" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:29" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A29" s="11">
         <v>9</v>
       </c>
@@ -6968,7 +6970,7 @@
         <v>-14.336526696129258</v>
       </c>
     </row>
-    <row r="30" spans="1:29" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:29" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A30" s="11">
         <v>9</v>
       </c>
@@ -7075,7 +7077,7 @@
         <v>2.2706632586558779</v>
       </c>
     </row>
-    <row r="31" spans="1:29" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:29" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A31" s="11">
         <v>9</v>
       </c>
@@ -7128,7 +7130,7 @@
       <c r="AB31" s="68"/>
       <c r="AC31" s="69"/>
     </row>
-    <row r="32" spans="1:29" s="63" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:29" s="63" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A32" s="56">
         <v>10</v>
       </c>
@@ -7163,7 +7165,7 @@
       <c r="AB32" s="71"/>
       <c r="AC32" s="70"/>
     </row>
-    <row r="33" spans="1:29" s="63" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:29" s="63" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A33" s="56">
         <v>10</v>
       </c>
@@ -7198,7 +7200,7 @@
       <c r="AB33" s="71"/>
       <c r="AC33" s="70"/>
     </row>
-    <row r="34" spans="1:29" s="63" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:29" s="63" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A34" s="56">
         <v>10</v>
       </c>
@@ -7233,7 +7235,7 @@
       <c r="AB34" s="71"/>
       <c r="AC34" s="70"/>
     </row>
-    <row r="35" spans="1:29" s="3" customFormat="1" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:29" s="3" customFormat="1" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="11">
         <v>11</v>
       </c>
@@ -7341,7 +7343,7 @@
         <v>-8.3544752539984337</v>
       </c>
     </row>
-    <row r="36" spans="1:29" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:29" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A36" s="11">
         <v>11</v>
       </c>
@@ -7449,7 +7451,7 @@
         <v>-21.868841080639719</v>
       </c>
     </row>
-    <row r="37" spans="1:29" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:29" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A37" s="11">
         <v>11</v>
       </c>
@@ -7502,7 +7504,7 @@
       <c r="AB37" s="68"/>
       <c r="AC37" s="69"/>
     </row>
-    <row r="38" spans="1:29" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:29" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A38" s="11">
         <v>12</v>
       </c>
@@ -7610,7 +7612,7 @@
         <v>-16.61247631773093</v>
       </c>
     </row>
-    <row r="39" spans="1:29" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:29" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A39" s="11">
         <v>12</v>
       </c>
@@ -7717,7 +7719,7 @@
         <v>7.1591847791813699</v>
       </c>
     </row>
-    <row r="40" spans="1:29" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:29" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A40" s="11">
         <v>12</v>
       </c>
@@ -7770,7 +7772,7 @@
       <c r="AB40" s="68"/>
       <c r="AC40" s="69"/>
     </row>
-    <row r="41" spans="1:29" s="63" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:29" s="63" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A41" s="56">
         <v>13</v>
       </c>
@@ -7805,7 +7807,7 @@
       <c r="AB41" s="71"/>
       <c r="AC41" s="70"/>
     </row>
-    <row r="42" spans="1:29" s="63" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:29" s="63" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A42" s="56">
         <v>13</v>
       </c>
@@ -7840,7 +7842,7 @@
       <c r="AB42" s="71"/>
       <c r="AC42" s="70"/>
     </row>
-    <row r="43" spans="1:29" s="63" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:29" s="63" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A43" s="56">
         <v>13</v>
       </c>
@@ -7875,7 +7877,7 @@
       <c r="AB43" s="71"/>
       <c r="AC43" s="70"/>
     </row>
-    <row r="44" spans="1:29" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:29" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A44" s="11">
         <v>14</v>
       </c>
@@ -7982,7 +7984,7 @@
         <v>13.253104495970366</v>
       </c>
     </row>
-    <row r="45" spans="1:29" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:29" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A45" s="11">
         <v>14</v>
       </c>
@@ -8089,7 +8091,7 @@
         <v>1.1003826370707486</v>
       </c>
     </row>
-    <row r="46" spans="1:29" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:29" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A46" s="11">
         <v>14</v>
       </c>
@@ -8142,7 +8144,7 @@
       <c r="AB46" s="68"/>
       <c r="AC46" s="69"/>
     </row>
-    <row r="47" spans="1:29" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:29" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A47" s="11">
         <v>15</v>
       </c>
@@ -8249,7 +8251,7 @@
         <v>-3.4725466114128736</v>
       </c>
     </row>
-    <row r="48" spans="1:29" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:29" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A48" s="11">
         <v>15</v>
       </c>
@@ -8356,7 +8358,7 @@
         <v>-3.1958196708118956</v>
       </c>
     </row>
-    <row r="49" spans="1:29" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:29" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A49" s="11">
         <v>15</v>
       </c>
@@ -8409,7 +8411,7 @@
       <c r="AB49" s="68"/>
       <c r="AC49" s="69"/>
     </row>
-    <row r="50" spans="1:29" s="63" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:29" s="63" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A50" s="56">
         <v>16</v>
       </c>
@@ -8444,7 +8446,7 @@
       <c r="AB50" s="71"/>
       <c r="AC50" s="70"/>
     </row>
-    <row r="51" spans="1:29" s="63" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:29" s="63" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A51" s="56">
         <v>16</v>
       </c>
@@ -8479,7 +8481,7 @@
       <c r="AB51" s="71"/>
       <c r="AC51" s="70"/>
     </row>
-    <row r="52" spans="1:29" s="63" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:29" s="63" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A52" s="56">
         <v>16</v>
       </c>
@@ -8514,7 +8516,7 @@
       <c r="AB52" s="71"/>
       <c r="AC52" s="70"/>
     </row>
-    <row r="53" spans="1:29" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:29" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A53" s="11">
         <v>17</v>
       </c>
@@ -8620,7 +8622,7 @@
         <v>-16.264590131535364</v>
       </c>
     </row>
-    <row r="54" spans="1:29" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:29" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A54" s="11">
         <v>17</v>
       </c>
@@ -8727,7 +8729,7 @@
         <v>-29.553798368804035</v>
       </c>
     </row>
-    <row r="55" spans="1:29" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:29" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A55" s="11">
         <v>17</v>
       </c>
@@ -8780,7 +8782,7 @@
       <c r="AB55" s="68"/>
       <c r="AC55" s="69"/>
     </row>
-    <row r="56" spans="1:29" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:29" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A56" s="11">
         <v>18</v>
       </c>
@@ -8888,7 +8890,7 @@
         <v>-16.645407002476105</v>
       </c>
     </row>
-    <row r="57" spans="1:29" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:29" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A57" s="11">
         <v>18</v>
       </c>
@@ -8995,7 +8997,7 @@
         <v>4.5839852879659198</v>
       </c>
     </row>
-    <row r="58" spans="1:29" s="3" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:29" s="3" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A58" s="11">
         <v>18</v>
       </c>
@@ -9159,12 +9161,12 @@
     <sheetView workbookViewId="2"/>
     <sheetView workbookViewId="3"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="11" max="86" width="8.85546875" style="3"/>
+    <col min="11" max="86" width="8.81640625" style="3"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:86" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:86" x14ac:dyDescent="0.35">
       <c r="C3" s="75" t="s">
         <v>6</v>
       </c>
@@ -9178,7 +9180,7 @@
       <c r="I3" s="75"/>
       <c r="J3" s="75"/>
     </row>
-    <row r="4" spans="1:86" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:86" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -9210,7 +9212,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:86" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:86" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
         <v>1</v>
       </c>
@@ -9300,7 +9302,7 @@
       <c r="CG5" s="3"/>
       <c r="CH5" s="3"/>
     </row>
-    <row r="6" spans="1:86" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:86" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="2">
         <v>2</v>
       </c>
@@ -9390,7 +9392,7 @@
       <c r="CG6" s="3"/>
       <c r="CH6" s="3"/>
     </row>
-    <row r="7" spans="1:86" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:86" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
         <v>3</v>
       </c>
@@ -9480,7 +9482,7 @@
       <c r="CG7" s="3"/>
       <c r="CH7" s="3"/>
     </row>
-    <row r="8" spans="1:86" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:86" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A8" s="2">
         <v>4</v>
       </c>
@@ -9570,7 +9572,7 @@
       <c r="CG8" s="3"/>
       <c r="CH8" s="3"/>
     </row>
-    <row r="9" spans="1:86" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:86" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="3">
         <v>5</v>
       </c>
@@ -9606,7 +9608,7 @@
         <v>480.3</v>
       </c>
     </row>
-    <row r="10" spans="1:86" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:86" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A10" s="3">
         <v>6</v>
       </c>
@@ -9642,7 +9644,7 @@
         <v>240.15</v>
       </c>
     </row>
-    <row r="11" spans="1:86" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:86" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A11" s="2">
         <v>7</v>
       </c>
@@ -9732,7 +9734,7 @@
       <c r="CG11" s="3"/>
       <c r="CH11" s="3"/>
     </row>
-    <row r="12" spans="1:86" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:86" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A12" s="3">
         <v>8</v>
       </c>
@@ -9768,7 +9770,7 @@
         <v>480.3</v>
       </c>
     </row>
-    <row r="13" spans="1:86" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:86" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A13" s="3">
         <v>9</v>
       </c>
@@ -9804,7 +9806,7 @@
         <v>240.15</v>
       </c>
     </row>
-    <row r="14" spans="1:86" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:86" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A14" s="2">
         <v>10</v>
       </c>
@@ -9894,7 +9896,7 @@
       <c r="CG14" s="3"/>
       <c r="CH14" s="3"/>
     </row>
-    <row r="15" spans="1:86" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:86" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A15" s="2">
         <v>11</v>
       </c>
@@ -9984,7 +9986,7 @@
       <c r="CG15" s="3"/>
       <c r="CH15" s="3"/>
     </row>
-    <row r="16" spans="1:86" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:86" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A16" s="3">
         <v>12</v>
       </c>
@@ -10020,7 +10022,7 @@
         <v>240.15</v>
       </c>
     </row>
-    <row r="17" spans="1:86" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:86" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A17" s="2">
         <v>13</v>
       </c>
@@ -10110,7 +10112,7 @@
       <c r="CG17" s="3"/>
       <c r="CH17" s="3"/>
     </row>
-    <row r="18" spans="1:86" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:86" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A18" s="3">
         <v>14</v>
       </c>
@@ -10146,7 +10148,7 @@
         <v>480.3</v>
       </c>
     </row>
-    <row r="19" spans="1:86" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:86" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A19" s="3">
         <v>15</v>
       </c>
@@ -10182,7 +10184,7 @@
         <v>240.15</v>
       </c>
     </row>
-    <row r="20" spans="1:86" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:86" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A20" s="2">
         <v>16</v>
       </c>
@@ -10272,7 +10274,7 @@
       <c r="CG20" s="3"/>
       <c r="CH20" s="3"/>
     </row>
-    <row r="21" spans="1:86" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:86" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A21" s="2">
         <v>17</v>
       </c>
@@ -10362,7 +10364,7 @@
       <c r="CG21" s="3"/>
       <c r="CH21" s="3"/>
     </row>
-    <row r="22" spans="1:86" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:86" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A22" s="3">
         <v>18</v>
       </c>
@@ -10398,7 +10400,7 @@
         <v>240.15</v>
       </c>
     </row>
-    <row r="27" spans="1:86" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:86" x14ac:dyDescent="0.35">
       <c r="H27" t="s">
         <v>12</v>
       </c>
@@ -10414,56 +10416,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10001</Type>
-    <SequenceNumber>1000</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10002</Type>
-    <SequenceNumber>1001</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10004</Type>
-    <SequenceNumber>1002</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10006</Type>
-    <SequenceNumber>1003</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-</spe:Receivers>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010013E660C0EEA2F44AA3B088C58E7762CB" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="5484fa9f9b42a97565e65fac7903a307">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="add409d8-c458-45bf-bf5f-710f0ed12ba3" xmlns:ns3="B9FBF822-0A65-4D1F-BC13-C27C7257EFA0" xmlns:ns4="b9fbf822-0a65-4d1f-bc13-c27c7257efa0" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="de45a4d41d0ddc6d7e8e18579ff54800" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="add409d8-c458-45bf-bf5f-710f0ed12ba3"/>
@@ -10730,7 +10682,66 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10001</Type>
+    <SequenceNumber>1000</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10002</Type>
+    <SequenceNumber>1001</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10004</Type>
+    <SequenceNumber>1002</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10006</Type>
+    <SequenceNumber>1003</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+</spe:Receivers>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <_dlc_DocId xmlns="add409d8-c458-45bf-bf5f-710f0ed12ba3">CY54R7KD54KC-91199970-192712</_dlc_DocId>
@@ -10744,24 +10755,7 @@
 </p:properties>
 </file>
 
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D23B5ADC-2FED-4856-AE1D-6D8A5A36E916}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E0D66368-F85C-4561-B8C5-570B6192D2BA}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -10781,7 +10775,23 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D23B5ADC-2FED-4856-AE1D-6D8A5A36E916}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{51CC3469-56E6-4BF6-AD20-3A6F9B943A35}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F80D695E-02F0-4FF4-A9B6-96C7E8E5A419}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -10790,12 +10800,4 @@
     <ds:schemaRef ds:uri="B9FBF822-0A65-4D1F-BC13-C27C7257EFA0"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{51CC3469-56E6-4BF6-AD20-3A6F9B943A35}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>